<commit_message>
1. Adding college and lab export successful
</commit_message>
<xml_diff>
--- a/data/standards/InputJSONData.xlsx
+++ b/data/standards/InputJSONData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\pw-openstudio-standards\data\standards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajszi\Documents\openstudio-standards\data\standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB54548-290B-4892-932C-14C45D77557D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD14F5B7-D88E-4E8D-8465-5C72AF0F0862}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="868" activeTab="4" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="4" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectInformation" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="251">
   <si>
     <t>Primary_Building_Type</t>
   </si>
@@ -728,6 +728,63 @@
   </si>
   <si>
     <t>Outpatient-Cafe</t>
+  </si>
+  <si>
+    <t>College-Conference</t>
+  </si>
+  <si>
+    <t>College-Corridor</t>
+  </si>
+  <si>
+    <t>College-ElevatorShaft</t>
+  </si>
+  <si>
+    <t>College-EnteranceLobby</t>
+  </si>
+  <si>
+    <t>College-Lounge</t>
+  </si>
+  <si>
+    <t>College-Office</t>
+  </si>
+  <si>
+    <t>College-Restroom</t>
+  </si>
+  <si>
+    <t>College-Utility</t>
+  </si>
+  <si>
+    <t>College-ArtClassroom</t>
+  </si>
+  <si>
+    <t>College-Classroom</t>
+  </si>
+  <si>
+    <t>College-Laboratory</t>
+  </si>
+  <si>
+    <t>College-LectureHall</t>
+  </si>
+  <si>
+    <t>College-MediaCenter</t>
+  </si>
+  <si>
+    <t>College-Stairs</t>
+  </si>
+  <si>
+    <t>College-Storage</t>
+  </si>
+  <si>
+    <t>Lab-Equipment_corridor</t>
+  </si>
+  <si>
+    <t>Lab-Lab_fumehood</t>
+  </si>
+  <si>
+    <t>Lab-Office</t>
+  </si>
+  <si>
+    <t>Lab-Open</t>
   </si>
 </sst>
 </file>
@@ -773,12 +830,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -870,7 +933,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -942,12 +1005,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -955,6 +1012,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -969,6 +1032,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1294,15 +1358,15 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -1312,7 +1376,7 @@
       </c>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1326,7 +1390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1340,7 +1404,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="6" t="s">
         <v>24</v>
@@ -1348,7 +1412,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>25</v>
@@ -1356,7 +1420,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -1364,7 +1428,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -1372,7 +1436,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -1380,7 +1444,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -1388,55 +1452,55 @@
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
@@ -1459,14 +1523,14 @@
       <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="9.109375" style="9"/>
-    <col min="8" max="16384" width="9.109375" style="7"/>
+    <col min="1" max="1" width="15.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9.140625" style="9"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1487,7 +1551,7 @@
       </c>
       <c r="G1" s="26"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1510,7 +1574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>150</v>
       </c>
@@ -1533,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1544,7 +1608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1555,7 +1619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1566,7 +1630,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1577,7 +1641,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1588,7 +1652,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1599,7 +1663,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1610,7 +1674,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1621,7 +1685,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1632,7 +1696,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1643,7 +1707,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1654,7 +1718,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1665,7 +1729,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1676,7 +1740,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1687,7 +1751,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1698,7 +1762,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1709,7 +1773,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1720,7 +1784,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1731,7 +1795,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1742,7 +1806,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1753,7 +1817,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1764,7 +1828,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1775,7 +1839,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1786,7 +1850,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1797,7 +1861,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1808,7 +1872,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1819,7 +1883,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1830,7 +1894,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1841,7 +1905,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1852,7 +1916,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1863,7 +1927,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1874,7 +1938,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1885,7 +1949,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1896,7 +1960,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1907,7 +1971,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1918,7 +1982,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1929,7 +1993,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1940,7 +2004,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1951,7 +2015,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1962,7 +2026,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1973,7 +2037,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1984,7 +2048,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1995,7 +2059,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2006,7 +2070,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2017,7 +2081,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -2028,7 +2092,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2039,7 +2103,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -2050,7 +2114,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -2061,7 +2125,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2072,7 +2136,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -2083,7 +2147,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -2094,7 +2158,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -2105,7 +2169,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -2116,7 +2180,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -2127,7 +2191,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -2138,7 +2202,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -2149,7 +2213,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -2160,7 +2224,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -2171,7 +2235,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -2182,7 +2246,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -2193,7 +2257,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -2204,7 +2268,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -2215,7 +2279,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -2226,7 +2290,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -2237,7 +2301,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -2248,7 +2312,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -2259,7 +2323,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -2270,7 +2334,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -2281,7 +2345,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -2292,7 +2356,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -2303,7 +2367,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -2331,59 +2395,59 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" style="9" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="36" max="38" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="39" max="40" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="38" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="66" max="16384" width="9.109375" style="9"/>
+    <col min="46" max="46" width="18.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="66" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
@@ -2395,76 +2459,76 @@
         <v>28</v>
       </c>
       <c r="E1" s="26"/>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="29" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="31"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="29"/>
       <c r="AO1" s="26" t="s">
         <v>32</v>
       </c>
       <c r="AP1" s="26"/>
-      <c r="AQ1" s="28" t="s">
+      <c r="AQ1" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="28"/>
-      <c r="AS1" s="28"/>
-      <c r="AT1" s="28"/>
-      <c r="AU1" s="28"/>
-      <c r="AV1" s="28"/>
-      <c r="AW1" s="28"/>
-      <c r="AX1" s="28"/>
-      <c r="AY1" s="28"/>
-      <c r="AZ1" s="28"/>
-      <c r="BA1" s="28"/>
-      <c r="BB1" s="28"/>
-      <c r="BC1" s="28"/>
-      <c r="BD1" s="28"/>
-      <c r="BE1" s="28"/>
-      <c r="BF1" s="28"/>
-      <c r="BG1" s="28"/>
-      <c r="BH1" s="28"/>
-      <c r="BI1" s="28"/>
-      <c r="BJ1" s="28"/>
-      <c r="BK1" s="28"/>
-      <c r="BL1" s="28"/>
-      <c r="BM1" s="28"/>
-    </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AR1" s="30"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="30"/>
+      <c r="AW1" s="30"/>
+      <c r="AX1" s="30"/>
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="30"/>
+      <c r="BF1" s="30"/>
+      <c r="BG1" s="30"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30"/>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2565,7 +2629,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>200000</v>
       </c>
@@ -2596,48 +2660,48 @@
       <c r="J3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="29" t="s">
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="29" t="s">
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="31"/>
-      <c r="Z3" s="29" t="s">
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="30"/>
-      <c r="AD3" s="31"/>
-      <c r="AE3" s="29" t="s">
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="29"/>
+      <c r="AE3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="AF3" s="30"/>
-      <c r="AG3" s="30"/>
-      <c r="AH3" s="30"/>
-      <c r="AI3" s="31"/>
-      <c r="AJ3" s="29" t="s">
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="28"/>
+      <c r="AH3" s="28"/>
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="AK3" s="30"/>
-      <c r="AL3" s="30"/>
-      <c r="AM3" s="30"/>
-      <c r="AN3" s="31"/>
+      <c r="AK3" s="28"/>
+      <c r="AL3" s="28"/>
+      <c r="AM3" s="28"/>
+      <c r="AN3" s="29"/>
       <c r="AO3" s="3">
         <v>0</v>
       </c>
@@ -2677,10 +2741,10 @@
       <c r="BA3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="BB3" s="27" t="s">
+      <c r="BB3" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BC3" s="27"/>
+      <c r="BC3" s="31"/>
       <c r="BD3" s="10" t="s">
         <v>57</v>
       </c>
@@ -2690,25 +2754,25 @@
       <c r="BF3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BG3" s="27" t="s">
+      <c r="BG3" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BH3" s="27"/>
+      <c r="BH3" s="31"/>
       <c r="BI3" s="10" t="s">
         <v>57</v>
       </c>
       <c r="BJ3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BK3" s="27" t="s">
+      <c r="BK3" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BL3" s="27"/>
+      <c r="BL3" s="31"/>
       <c r="BM3" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
@@ -2734,57 +2798,57 @@
       <c r="K4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="29" t="s">
+      <c r="L4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="31"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="29"/>
       <c r="P4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="29" t="s">
+      <c r="Q4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="31"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="29"/>
       <c r="U4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="29" t="s">
+      <c r="V4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="31"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="29"/>
       <c r="Z4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AA4" s="29" t="s">
+      <c r="AA4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="31"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="29"/>
       <c r="AE4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AF4" s="29" t="s">
+      <c r="AF4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AG4" s="30"/>
-      <c r="AH4" s="30"/>
-      <c r="AI4" s="31"/>
+      <c r="AG4" s="28"/>
+      <c r="AH4" s="28"/>
+      <c r="AI4" s="29"/>
       <c r="AJ4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AK4" s="29" t="s">
+      <c r="AK4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AL4" s="30"/>
-      <c r="AM4" s="30"/>
-      <c r="AN4" s="31"/>
+      <c r="AL4" s="28"/>
+      <c r="AM4" s="28"/>
+      <c r="AN4" s="29"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3">
         <v>5</v>
@@ -2859,7 +2923,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="5"/>
       <c r="C5" s="3">
@@ -3028,7 +3092,7 @@
       </c>
       <c r="BM5" s="10"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
@@ -3159,7 +3223,7 @@
       </c>
       <c r="BM6" s="10"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -3276,7 +3340,7 @@
       </c>
       <c r="BM7" s="10"/>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -3381,7 +3445,7 @@
       </c>
       <c r="BM8" s="10"/>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="3">
@@ -3484,7 +3548,7 @@
       </c>
       <c r="BM9" s="10"/>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -3581,7 +3645,7 @@
       <c r="BL10" s="3"/>
       <c r="BM10" s="3"/>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -3678,7 +3742,7 @@
       <c r="BL11" s="3"/>
       <c r="BM11" s="3"/>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="3">
@@ -3775,7 +3839,7 @@
       <c r="BL12" s="3"/>
       <c r="BM12" s="3"/>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -3872,7 +3936,7 @@
       <c r="BL13" s="3"/>
       <c r="BM13" s="3"/>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3">
@@ -3969,7 +4033,7 @@
       <c r="BL14" s="3"/>
       <c r="BM14" s="3"/>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
@@ -4066,7 +4130,7 @@
       <c r="BL15" s="3"/>
       <c r="BM15" s="3"/>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3">
@@ -4163,7 +4227,7 @@
       <c r="BL16" s="3"/>
       <c r="BM16" s="3"/>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
@@ -4260,7 +4324,7 @@
       <c r="BL17" s="3"/>
       <c r="BM17" s="3"/>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3">
@@ -4357,7 +4421,7 @@
       <c r="BL18" s="3"/>
       <c r="BM18" s="3"/>
     </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3">
@@ -4454,7 +4518,7 @@
       <c r="BL19" s="3"/>
       <c r="BM19" s="3"/>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3">
@@ -4527,7 +4591,7 @@
       <c r="BL20" s="3"/>
       <c r="BM20" s="3"/>
     </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3">
@@ -4600,7 +4664,7 @@
       <c r="BL21" s="3"/>
       <c r="BM21" s="3"/>
     </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3">
@@ -4673,7 +4737,7 @@
       <c r="BL22" s="3"/>
       <c r="BM22" s="3"/>
     </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3">
@@ -4746,7 +4810,7 @@
       <c r="BL23" s="3"/>
       <c r="BM23" s="3"/>
     </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3">
@@ -4819,7 +4883,7 @@
       <c r="BL24" s="3"/>
       <c r="BM24" s="3"/>
     </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3">
@@ -4892,7 +4956,7 @@
       <c r="BL25" s="3"/>
       <c r="BM25" s="3"/>
     </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3">
@@ -4965,7 +5029,7 @@
       <c r="BL26" s="3"/>
       <c r="BM26" s="3"/>
     </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3">
@@ -5038,7 +5102,7 @@
       <c r="BL27" s="3"/>
       <c r="BM27" s="3"/>
     </row>
-    <row r="28" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3">
@@ -5111,7 +5175,7 @@
       <c r="BL28" s="3"/>
       <c r="BM28" s="3"/>
     </row>
-    <row r="29" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3">
@@ -5184,7 +5248,7 @@
       <c r="BL29" s="3"/>
       <c r="BM29" s="3"/>
     </row>
-    <row r="30" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3">
@@ -5257,7 +5321,7 @@
       <c r="BL30" s="3"/>
       <c r="BM30" s="3"/>
     </row>
-    <row r="31" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3">
@@ -5330,7 +5394,7 @@
       <c r="BL31" s="3"/>
       <c r="BM31" s="3"/>
     </row>
-    <row r="32" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3">
@@ -5403,7 +5467,7 @@
       <c r="BL32" s="3"/>
       <c r="BM32" s="3"/>
     </row>
-    <row r="33" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3">
@@ -5476,7 +5540,7 @@
       <c r="BL33" s="3"/>
       <c r="BM33" s="3"/>
     </row>
-    <row r="34" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3">
@@ -5549,7 +5613,7 @@
       <c r="BL34" s="3"/>
       <c r="BM34" s="3"/>
     </row>
-    <row r="35" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3">
@@ -5622,7 +5686,7 @@
       <c r="BL35" s="3"/>
       <c r="BM35" s="3"/>
     </row>
-    <row r="36" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3">
@@ -5693,7 +5757,7 @@
       <c r="BL36" s="3"/>
       <c r="BM36" s="3"/>
     </row>
-    <row r="37" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3">
@@ -5764,7 +5828,7 @@
       <c r="BL37" s="3"/>
       <c r="BM37" s="3"/>
     </row>
-    <row r="38" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3">
@@ -5835,7 +5899,7 @@
       <c r="BL38" s="3"/>
       <c r="BM38" s="3"/>
     </row>
-    <row r="39" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3">
@@ -5906,7 +5970,7 @@
       <c r="BL39" s="3"/>
       <c r="BM39" s="3"/>
     </row>
-    <row r="40" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3">
@@ -5977,7 +6041,7 @@
       <c r="BL40" s="3"/>
       <c r="BM40" s="3"/>
     </row>
-    <row r="41" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3">
@@ -6048,7 +6112,7 @@
       <c r="BL41" s="3"/>
       <c r="BM41" s="3"/>
     </row>
-    <row r="42" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3">
@@ -6119,7 +6183,7 @@
       <c r="BL42" s="3"/>
       <c r="BM42" s="3"/>
     </row>
-    <row r="43" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3">
@@ -6190,7 +6254,7 @@
       <c r="BL43" s="3"/>
       <c r="BM43" s="3"/>
     </row>
-    <row r="44" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3">
@@ -6261,7 +6325,7 @@
       <c r="BL44" s="3"/>
       <c r="BM44" s="3"/>
     </row>
-    <row r="45" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3">
@@ -6332,7 +6396,7 @@
       <c r="BL45" s="3"/>
       <c r="BM45" s="3"/>
     </row>
-    <row r="46" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3">
@@ -6403,7 +6467,7 @@
       <c r="BL46" s="3"/>
       <c r="BM46" s="3"/>
     </row>
-    <row r="47" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3">
@@ -6474,7 +6538,7 @@
       <c r="BL47" s="3"/>
       <c r="BM47" s="3"/>
     </row>
-    <row r="48" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3">
@@ -6545,7 +6609,7 @@
       <c r="BL48" s="3"/>
       <c r="BM48" s="3"/>
     </row>
-    <row r="49" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3">
@@ -6616,7 +6680,7 @@
       <c r="BL49" s="3"/>
       <c r="BM49" s="3"/>
     </row>
-    <row r="50" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3">
@@ -6687,7 +6751,7 @@
       <c r="BL50" s="3"/>
       <c r="BM50" s="3"/>
     </row>
-    <row r="51" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3">
@@ -6758,7 +6822,7 @@
       <c r="BL51" s="3"/>
       <c r="BM51" s="3"/>
     </row>
-    <row r="52" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3">
@@ -6829,7 +6893,7 @@
       <c r="BL52" s="3"/>
       <c r="BM52" s="3"/>
     </row>
-    <row r="53" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -6898,7 +6962,7 @@
       <c r="BL53" s="3"/>
       <c r="BM53" s="3"/>
     </row>
-    <row r="54" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -6967,7 +7031,7 @@
       <c r="BL54" s="3"/>
       <c r="BM54" s="3"/>
     </row>
-    <row r="55" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -7036,7 +7100,7 @@
       <c r="BL55" s="3"/>
       <c r="BM55" s="3"/>
     </row>
-    <row r="56" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -7105,7 +7169,7 @@
       <c r="BL56" s="3"/>
       <c r="BM56" s="3"/>
     </row>
-    <row r="57" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -7174,7 +7238,7 @@
       <c r="BL57" s="3"/>
       <c r="BM57" s="3"/>
     </row>
-    <row r="58" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -7243,7 +7307,7 @@
       <c r="BL58" s="3"/>
       <c r="BM58" s="3"/>
     </row>
-    <row r="59" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -7312,7 +7376,7 @@
       <c r="BL59" s="3"/>
       <c r="BM59" s="3"/>
     </row>
-    <row r="60" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -7381,7 +7445,7 @@
       <c r="BL60" s="3"/>
       <c r="BM60" s="3"/>
     </row>
-    <row r="61" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -7450,7 +7514,7 @@
       <c r="BL61" s="3"/>
       <c r="BM61" s="3"/>
     </row>
-    <row r="62" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -7519,7 +7583,7 @@
       <c r="BL62" s="3"/>
       <c r="BM62" s="3"/>
     </row>
-    <row r="63" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -7588,7 +7652,7 @@
       <c r="BL63" s="3"/>
       <c r="BM63" s="3"/>
     </row>
-    <row r="64" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -7657,7 +7721,7 @@
       <c r="BL64" s="3"/>
       <c r="BM64" s="3"/>
     </row>
-    <row r="65" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -7726,7 +7790,7 @@
       <c r="BL65" s="3"/>
       <c r="BM65" s="3"/>
     </row>
-    <row r="66" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -7795,7 +7859,7 @@
       <c r="BL66" s="3"/>
       <c r="BM66" s="3"/>
     </row>
-    <row r="67" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -7864,7 +7928,7 @@
       <c r="BL67" s="3"/>
       <c r="BM67" s="3"/>
     </row>
-    <row r="68" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -7933,7 +7997,7 @@
       <c r="BL68" s="3"/>
       <c r="BM68" s="3"/>
     </row>
-    <row r="69" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -8002,7 +8066,7 @@
       <c r="BL69" s="3"/>
       <c r="BM69" s="3"/>
     </row>
-    <row r="70" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -8071,7 +8135,7 @@
       <c r="BL70" s="3"/>
       <c r="BM70" s="3"/>
     </row>
-    <row r="71" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -8140,7 +8204,7 @@
       <c r="BL71" s="3"/>
       <c r="BM71" s="3"/>
     </row>
-    <row r="72" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -8209,7 +8273,7 @@
       <c r="BL72" s="3"/>
       <c r="BM72" s="3"/>
     </row>
-    <row r="73" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -8278,7 +8342,7 @@
       <c r="BL73" s="3"/>
       <c r="BM73" s="3"/>
     </row>
-    <row r="74" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -8347,11 +8411,11 @@
       <c r="BL74" s="3"/>
       <c r="BM74" s="3"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D142" s="8"/>
       <c r="E142" s="8"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="8"/>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
@@ -8365,6 +8429,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="AQ2:AV2"/>
+    <mergeCell ref="AW2:BC2"/>
+    <mergeCell ref="BD2:BH2"/>
+    <mergeCell ref="BI2:BL2"/>
+    <mergeCell ref="BB3:BC3"/>
+    <mergeCell ref="AQ1:BM1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I1:AN1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="AO1:AP1"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="N5:O5"/>
@@ -8381,23 +8462,6 @@
     <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="AE3:AI3"/>
     <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AQ1:BM1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I1:AN1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="BG3:BH3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="AQ2:AV2"/>
-    <mergeCell ref="AW2:BC2"/>
-    <mergeCell ref="BD2:BH2"/>
-    <mergeCell ref="BI2:BL2"/>
-    <mergeCell ref="BB3:BC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -8412,21 +8476,21 @@
       <selection activeCell="J23" sqref="A23:J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="9" customWidth="1"/>
-    <col min="5" max="6" width="9.109375" style="9"/>
-    <col min="7" max="7" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="9" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="9"/>
+    <col min="7" max="7" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="7"/>
+    <col min="11" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>80</v>
       </c>
@@ -8448,7 +8512,7 @@
       </c>
       <c r="J1" s="32"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8480,7 +8544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>40</v>
       </c>
@@ -8520,7 +8584,7 @@
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>5</v>
@@ -8543,7 +8607,7 @@
       </c>
       <c r="R4" s="9"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>10</v>
@@ -8565,7 +8629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>15</v>
@@ -8587,7 +8651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>20</v>
@@ -8609,7 +8673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>25</v>
@@ -8631,7 +8695,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>30</v>
@@ -8653,7 +8717,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>35</v>
@@ -8675,7 +8739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>40</v>
@@ -8697,7 +8761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>45</v>
@@ -8719,7 +8783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>50</v>
@@ -8741,7 +8805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>55</v>
@@ -8764,7 +8828,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>60</v>
@@ -8791,7 +8855,7 @@
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>65</v>
@@ -8813,7 +8877,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>70</v>
@@ -8835,7 +8899,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>75</v>
@@ -8857,7 +8921,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>80</v>
@@ -8890,7 +8954,7 @@
       <c r="T19" s="14"/>
       <c r="U19" s="14"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>85</v>
@@ -8910,7 +8974,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>90</v>
@@ -8930,7 +8994,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>95</v>
@@ -8950,7 +9014,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -8966,55 +9030,55 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="14"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="14"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="14"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="14"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="14"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="14"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="14"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="14"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="14"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="14"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="14"/>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="14"/>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="14"/>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="14"/>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="14"/>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="14"/>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="14"/>
     </row>
   </sheetData>
@@ -9032,26 +9096,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C609DAD-BC63-4626-ACCC-69F8C32CB7AB}">
-  <dimension ref="A1:B127"/>
+  <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B148" sqref="A146:B148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="7"/>
+    <col min="1" max="1" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="31"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="29"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -9059,7 +9123,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -9067,748 +9131,874 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="18" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="18" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="18" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="18" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="18" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="18" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="18" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="18" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="18" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="18" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="18" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="18" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="18" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="18" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="18" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="18" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="18" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="18" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="18" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="18" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="18" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="18" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="18" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="18" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="18" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="18" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="18" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="18" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="18" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="18" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="18" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="18" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="18" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="18" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="18" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="18" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="18" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="18" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="18" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="18" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="18" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="18" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="18" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="18" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="18" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="18" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="18" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="18" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="18" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="18" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="18" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="18" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="18" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="18" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="18" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="18" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="18" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="18" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="18" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="18" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="18" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="18" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="18" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="18" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="18" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="18" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="18" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="18" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="18" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="18" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="18" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="18" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="18" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="18" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="18" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="18" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="18" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="18" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="18" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="18" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="18" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="16"/>
       <c r="B103" s="18" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="16"/>
       <c r="B104" s="18" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="16"/>
       <c r="B105" s="18" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="16"/>
       <c r="B106" s="18" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="16"/>
       <c r="B107" s="18" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="16"/>
       <c r="B108" s="18" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="16"/>
       <c r="B109" s="18" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="16"/>
       <c r="B110" s="18" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="16"/>
       <c r="B111" s="18" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="16"/>
       <c r="B112" s="18" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="16"/>
       <c r="B113" s="18" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="16"/>
       <c r="B114" s="18" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="16"/>
       <c r="B115" s="18" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="16"/>
       <c r="B116" s="18" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="16"/>
       <c r="B117" s="18" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="16"/>
       <c r="B118" s="18" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="16"/>
       <c r="B119" s="18" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="16"/>
       <c r="B120" s="18" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="16"/>
       <c r="B121" s="18" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="16"/>
       <c r="B122" s="18" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="16"/>
       <c r="B123" s="18" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="16"/>
       <c r="B124" s="18" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="16"/>
       <c r="B125" s="18" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="16"/>
       <c r="B126" s="18" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="16"/>
       <c r="B127" s="18" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="16"/>
+      <c r="B128" s="36" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="16"/>
+      <c r="B129" s="36" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="16"/>
+      <c r="B130" s="36" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="16"/>
+      <c r="B131" s="36" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="16"/>
+      <c r="B132" s="36" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="16"/>
+      <c r="B133" s="36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="16"/>
+      <c r="B134" s="36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="16"/>
+      <c r="B135" s="36" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="16"/>
+      <c r="B136" s="36" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="16"/>
+      <c r="B137" s="36" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="16"/>
+      <c r="B138" s="36" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="16"/>
+      <c r="B139" s="36" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="16"/>
+      <c r="B140" s="36" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="16"/>
+      <c r="B141" s="36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="16"/>
+      <c r="B142" s="36" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="16"/>
+      <c r="B143" s="36" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="16"/>
+      <c r="B144" s="36" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="16"/>
+      <c r="B145" s="36" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="16"/>
+      <c r="B146" s="36" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="16"/>
+      <c r="B147" s="36" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="16"/>
+      <c r="B148" s="36" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -9828,24 +10018,24 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="7"/>
+    <col min="1" max="1" width="43.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -9861,7 +10051,7 @@
       </c>
       <c r="F2" s="35"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>98</v>
       </c>
@@ -9881,7 +10071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="15" t="s">
         <v>92</v>
@@ -9899,7 +10089,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="15" t="s">
         <v>93</v>
@@ -9913,7 +10103,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="15" t="s">
         <v>94</v>
@@ -9927,7 +10117,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="15" t="s">
         <v>95</v>
@@ -9941,7 +10131,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="15" t="s">
         <v>96</v>
@@ -9955,7 +10145,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="15" t="s">
         <v>97</v>
@@ -9969,7 +10159,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="15" t="s">
         <v>98</v>
@@ -9979,7 +10169,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="15" t="s">
         <v>99</v>
@@ -9989,7 +10179,7 @@
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="15" t="s">
         <v>100</v>
@@ -9999,7 +10189,7 @@
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="16" t="s">
         <v>228</v>
@@ -10028,21 +10218,21 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="7"/>
+    <col min="1" max="1" width="19.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>87</v>
       </c>
       <c r="B1" s="26"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -10050,7 +10240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -10058,7 +10248,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>89</v>
@@ -10080,20 +10270,20 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="9"/>
-    <col min="3" max="16384" width="9.109375" style="7"/>
+    <col min="1" max="1" width="11.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="9"/>
+    <col min="3" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="26"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -10101,7 +10291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>50</v>
       </c>
@@ -10109,115 +10299,115 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3">
         <v>100</v>

</xml_diff>

<commit_message>
Fix for incorrect HVAC name PSZ-HP with Gas Auxiliary Heating to PSZ-HP with Electric Auxiliary Heating
</commit_message>
<xml_diff>
--- a/data/standards/InputJSONData.xlsx
+++ b/data/standards/InputJSONData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\pw-openstudio-standards\data\standards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajszi\Documents\openstudio-standards\data\standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB54548-290B-4892-932C-14C45D77557D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E9685D-130A-4F3E-886E-65799BD08870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="868" activeTab="4" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="5" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectInformation" sheetId="1" r:id="rId1"/>
@@ -319,9 +319,6 @@
     <t>PSZ-AC with Gas Heating</t>
   </si>
   <si>
-    <t>PSZ-HP with Gas Auxiliary Heating</t>
-  </si>
-  <si>
     <t>Fan Coils with Water-Cooled Chiller and Boiler HW Heating</t>
   </si>
   <si>
@@ -728,6 +725,9 @@
   </si>
   <si>
     <t>Outpatient-Cafe</t>
+  </si>
+  <si>
+    <t>PSZ-HP with Electric Auxiliary Heating</t>
   </si>
 </sst>
 </file>
@@ -771,6 +771,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -942,12 +943,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -955,6 +950,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1294,25 +1295,25 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1326,7 +1327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1334,13 +1335,13 @@
         <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="6" t="s">
         <v>24</v>
@@ -1348,7 +1349,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>25</v>
@@ -1356,7 +1357,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -1364,7 +1365,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -1372,7 +1373,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -1380,7 +1381,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -1388,55 +1389,55 @@
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
@@ -1459,14 +1460,14 @@
       <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="9.109375" style="9"/>
-    <col min="8" max="16384" width="9.109375" style="7"/>
+    <col min="1" max="1" width="15.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9.140625" style="9"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1487,7 +1488,7 @@
       </c>
       <c r="G1" s="26"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1510,7 +1511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>150</v>
       </c>
@@ -1533,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1544,7 +1545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1555,7 +1556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1566,7 +1567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1577,7 +1578,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1588,7 +1589,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1599,7 +1600,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1610,7 +1611,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1621,7 +1622,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1632,7 +1633,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1643,7 +1644,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1654,7 +1655,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1665,7 +1666,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1676,7 +1677,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1687,7 +1688,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1698,7 +1699,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1709,7 +1710,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1720,7 +1721,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1731,7 +1732,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1742,7 +1743,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1753,7 +1754,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1764,7 +1765,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1775,7 +1776,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1786,7 +1787,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1797,7 +1798,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1808,7 +1809,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1819,7 +1820,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1830,7 +1831,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1841,7 +1842,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1852,7 +1853,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1863,7 +1864,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1874,7 +1875,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1885,7 +1886,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1896,7 +1897,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1907,7 +1908,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1918,7 +1919,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1929,7 +1930,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1940,7 +1941,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1951,7 +1952,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1962,7 +1963,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1973,7 +1974,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1984,7 +1985,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1995,7 +1996,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2006,7 +2007,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2017,7 +2018,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -2028,7 +2029,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2039,7 +2040,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -2050,7 +2051,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -2061,7 +2062,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2072,7 +2073,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -2083,7 +2084,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -2094,7 +2095,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -2105,7 +2106,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -2116,7 +2117,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -2127,7 +2128,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -2138,7 +2139,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -2149,7 +2150,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -2160,7 +2161,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -2171,7 +2172,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -2182,7 +2183,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -2193,7 +2194,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -2204,7 +2205,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -2215,7 +2216,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -2226,7 +2227,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -2237,7 +2238,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -2248,7 +2249,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -2259,7 +2260,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -2270,7 +2271,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -2281,7 +2282,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -2292,7 +2293,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -2303,7 +2304,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -2331,59 +2332,59 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" style="9" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="36" max="38" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="39" max="40" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="38" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="66" max="16384" width="9.109375" style="9"/>
+    <col min="46" max="46" width="18.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="66" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
@@ -2395,76 +2396,76 @@
         <v>28</v>
       </c>
       <c r="E1" s="26"/>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="29" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="31"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="29"/>
       <c r="AO1" s="26" t="s">
         <v>32</v>
       </c>
       <c r="AP1" s="26"/>
-      <c r="AQ1" s="28" t="s">
+      <c r="AQ1" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="28"/>
-      <c r="AS1" s="28"/>
-      <c r="AT1" s="28"/>
-      <c r="AU1" s="28"/>
-      <c r="AV1" s="28"/>
-      <c r="AW1" s="28"/>
-      <c r="AX1" s="28"/>
-      <c r="AY1" s="28"/>
-      <c r="AZ1" s="28"/>
-      <c r="BA1" s="28"/>
-      <c r="BB1" s="28"/>
-      <c r="BC1" s="28"/>
-      <c r="BD1" s="28"/>
-      <c r="BE1" s="28"/>
-      <c r="BF1" s="28"/>
-      <c r="BG1" s="28"/>
-      <c r="BH1" s="28"/>
-      <c r="BI1" s="28"/>
-      <c r="BJ1" s="28"/>
-      <c r="BK1" s="28"/>
-      <c r="BL1" s="28"/>
-      <c r="BM1" s="28"/>
-    </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AR1" s="30"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="30"/>
+      <c r="AW1" s="30"/>
+      <c r="AX1" s="30"/>
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="30"/>
+      <c r="BF1" s="30"/>
+      <c r="BG1" s="30"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30"/>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2485,7 +2486,7 @@
       </c>
       <c r="G2" s="26"/>
       <c r="H2" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>1</v>
@@ -2565,7 +2566,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>200000</v>
       </c>
@@ -2596,48 +2597,48 @@
       <c r="J3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="29" t="s">
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="29" t="s">
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="31"/>
-      <c r="Z3" s="29" t="s">
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="30"/>
-      <c r="AD3" s="31"/>
-      <c r="AE3" s="29" t="s">
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="29"/>
+      <c r="AE3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="AF3" s="30"/>
-      <c r="AG3" s="30"/>
-      <c r="AH3" s="30"/>
-      <c r="AI3" s="31"/>
-      <c r="AJ3" s="29" t="s">
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="28"/>
+      <c r="AH3" s="28"/>
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="AK3" s="30"/>
-      <c r="AL3" s="30"/>
-      <c r="AM3" s="30"/>
-      <c r="AN3" s="31"/>
+      <c r="AK3" s="28"/>
+      <c r="AL3" s="28"/>
+      <c r="AM3" s="28"/>
+      <c r="AN3" s="29"/>
       <c r="AO3" s="3">
         <v>0</v>
       </c>
@@ -2677,10 +2678,10 @@
       <c r="BA3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="BB3" s="27" t="s">
+      <c r="BB3" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BC3" s="27"/>
+      <c r="BC3" s="31"/>
       <c r="BD3" s="10" t="s">
         <v>57</v>
       </c>
@@ -2690,25 +2691,25 @@
       <c r="BF3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BG3" s="27" t="s">
+      <c r="BG3" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BH3" s="27"/>
+      <c r="BH3" s="31"/>
       <c r="BI3" s="10" t="s">
         <v>57</v>
       </c>
       <c r="BJ3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BK3" s="27" t="s">
+      <c r="BK3" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BL3" s="27"/>
+      <c r="BL3" s="31"/>
       <c r="BM3" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
@@ -2734,57 +2735,57 @@
       <c r="K4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="29" t="s">
+      <c r="L4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="31"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="29"/>
       <c r="P4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="29" t="s">
+      <c r="Q4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="31"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="29"/>
       <c r="U4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="29" t="s">
+      <c r="V4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="31"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="29"/>
       <c r="Z4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AA4" s="29" t="s">
+      <c r="AA4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="31"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="29"/>
       <c r="AE4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AF4" s="29" t="s">
+      <c r="AF4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AG4" s="30"/>
-      <c r="AH4" s="30"/>
-      <c r="AI4" s="31"/>
+      <c r="AG4" s="28"/>
+      <c r="AH4" s="28"/>
+      <c r="AI4" s="29"/>
       <c r="AJ4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AK4" s="29" t="s">
+      <c r="AK4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AL4" s="30"/>
-      <c r="AM4" s="30"/>
-      <c r="AN4" s="31"/>
+      <c r="AL4" s="28"/>
+      <c r="AM4" s="28"/>
+      <c r="AN4" s="29"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3">
         <v>5</v>
@@ -2859,7 +2860,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="5"/>
       <c r="C5" s="3">
@@ -3028,7 +3029,7 @@
       </c>
       <c r="BM5" s="10"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
@@ -3159,7 +3160,7 @@
       </c>
       <c r="BM6" s="10"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -3276,7 +3277,7 @@
       </c>
       <c r="BM7" s="10"/>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -3381,7 +3382,7 @@
       </c>
       <c r="BM8" s="10"/>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="3">
@@ -3484,7 +3485,7 @@
       </c>
       <c r="BM9" s="10"/>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -3581,7 +3582,7 @@
       <c r="BL10" s="3"/>
       <c r="BM10" s="3"/>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -3678,7 +3679,7 @@
       <c r="BL11" s="3"/>
       <c r="BM11" s="3"/>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="3">
@@ -3775,7 +3776,7 @@
       <c r="BL12" s="3"/>
       <c r="BM12" s="3"/>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -3872,7 +3873,7 @@
       <c r="BL13" s="3"/>
       <c r="BM13" s="3"/>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3">
@@ -3969,7 +3970,7 @@
       <c r="BL14" s="3"/>
       <c r="BM14" s="3"/>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
@@ -4066,7 +4067,7 @@
       <c r="BL15" s="3"/>
       <c r="BM15" s="3"/>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3">
@@ -4163,7 +4164,7 @@
       <c r="BL16" s="3"/>
       <c r="BM16" s="3"/>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
@@ -4260,7 +4261,7 @@
       <c r="BL17" s="3"/>
       <c r="BM17" s="3"/>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3">
@@ -4357,7 +4358,7 @@
       <c r="BL18" s="3"/>
       <c r="BM18" s="3"/>
     </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3">
@@ -4454,7 +4455,7 @@
       <c r="BL19" s="3"/>
       <c r="BM19" s="3"/>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3">
@@ -4527,7 +4528,7 @@
       <c r="BL20" s="3"/>
       <c r="BM20" s="3"/>
     </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3">
@@ -4600,7 +4601,7 @@
       <c r="BL21" s="3"/>
       <c r="BM21" s="3"/>
     </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3">
@@ -4673,7 +4674,7 @@
       <c r="BL22" s="3"/>
       <c r="BM22" s="3"/>
     </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3">
@@ -4746,7 +4747,7 @@
       <c r="BL23" s="3"/>
       <c r="BM23" s="3"/>
     </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3">
@@ -4819,7 +4820,7 @@
       <c r="BL24" s="3"/>
       <c r="BM24" s="3"/>
     </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3">
@@ -4892,7 +4893,7 @@
       <c r="BL25" s="3"/>
       <c r="BM25" s="3"/>
     </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3">
@@ -4965,7 +4966,7 @@
       <c r="BL26" s="3"/>
       <c r="BM26" s="3"/>
     </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3">
@@ -5038,7 +5039,7 @@
       <c r="BL27" s="3"/>
       <c r="BM27" s="3"/>
     </row>
-    <row r="28" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3">
@@ -5111,7 +5112,7 @@
       <c r="BL28" s="3"/>
       <c r="BM28" s="3"/>
     </row>
-    <row r="29" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3">
@@ -5184,7 +5185,7 @@
       <c r="BL29" s="3"/>
       <c r="BM29" s="3"/>
     </row>
-    <row r="30" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3">
@@ -5257,7 +5258,7 @@
       <c r="BL30" s="3"/>
       <c r="BM30" s="3"/>
     </row>
-    <row r="31" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3">
@@ -5330,7 +5331,7 @@
       <c r="BL31" s="3"/>
       <c r="BM31" s="3"/>
     </row>
-    <row r="32" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3">
@@ -5403,7 +5404,7 @@
       <c r="BL32" s="3"/>
       <c r="BM32" s="3"/>
     </row>
-    <row r="33" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3">
@@ -5476,7 +5477,7 @@
       <c r="BL33" s="3"/>
       <c r="BM33" s="3"/>
     </row>
-    <row r="34" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3">
@@ -5549,7 +5550,7 @@
       <c r="BL34" s="3"/>
       <c r="BM34" s="3"/>
     </row>
-    <row r="35" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3">
@@ -5622,7 +5623,7 @@
       <c r="BL35" s="3"/>
       <c r="BM35" s="3"/>
     </row>
-    <row r="36" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3">
@@ -5693,7 +5694,7 @@
       <c r="BL36" s="3"/>
       <c r="BM36" s="3"/>
     </row>
-    <row r="37" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3">
@@ -5764,7 +5765,7 @@
       <c r="BL37" s="3"/>
       <c r="BM37" s="3"/>
     </row>
-    <row r="38" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3">
@@ -5835,7 +5836,7 @@
       <c r="BL38" s="3"/>
       <c r="BM38" s="3"/>
     </row>
-    <row r="39" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3">
@@ -5906,7 +5907,7 @@
       <c r="BL39" s="3"/>
       <c r="BM39" s="3"/>
     </row>
-    <row r="40" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3">
@@ -5977,7 +5978,7 @@
       <c r="BL40" s="3"/>
       <c r="BM40" s="3"/>
     </row>
-    <row r="41" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3">
@@ -6048,7 +6049,7 @@
       <c r="BL41" s="3"/>
       <c r="BM41" s="3"/>
     </row>
-    <row r="42" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3">
@@ -6119,7 +6120,7 @@
       <c r="BL42" s="3"/>
       <c r="BM42" s="3"/>
     </row>
-    <row r="43" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3">
@@ -6190,7 +6191,7 @@
       <c r="BL43" s="3"/>
       <c r="BM43" s="3"/>
     </row>
-    <row r="44" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3">
@@ -6261,7 +6262,7 @@
       <c r="BL44" s="3"/>
       <c r="BM44" s="3"/>
     </row>
-    <row r="45" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3">
@@ -6332,7 +6333,7 @@
       <c r="BL45" s="3"/>
       <c r="BM45" s="3"/>
     </row>
-    <row r="46" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3">
@@ -6403,7 +6404,7 @@
       <c r="BL46" s="3"/>
       <c r="BM46" s="3"/>
     </row>
-    <row r="47" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3">
@@ -6474,7 +6475,7 @@
       <c r="BL47" s="3"/>
       <c r="BM47" s="3"/>
     </row>
-    <row r="48" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3">
@@ -6545,7 +6546,7 @@
       <c r="BL48" s="3"/>
       <c r="BM48" s="3"/>
     </row>
-    <row r="49" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3">
@@ -6616,7 +6617,7 @@
       <c r="BL49" s="3"/>
       <c r="BM49" s="3"/>
     </row>
-    <row r="50" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3">
@@ -6687,7 +6688,7 @@
       <c r="BL50" s="3"/>
       <c r="BM50" s="3"/>
     </row>
-    <row r="51" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3">
@@ -6758,7 +6759,7 @@
       <c r="BL51" s="3"/>
       <c r="BM51" s="3"/>
     </row>
-    <row r="52" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3">
@@ -6829,7 +6830,7 @@
       <c r="BL52" s="3"/>
       <c r="BM52" s="3"/>
     </row>
-    <row r="53" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -6898,7 +6899,7 @@
       <c r="BL53" s="3"/>
       <c r="BM53" s="3"/>
     </row>
-    <row r="54" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -6967,7 +6968,7 @@
       <c r="BL54" s="3"/>
       <c r="BM54" s="3"/>
     </row>
-    <row r="55" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -7036,7 +7037,7 @@
       <c r="BL55" s="3"/>
       <c r="BM55" s="3"/>
     </row>
-    <row r="56" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -7105,7 +7106,7 @@
       <c r="BL56" s="3"/>
       <c r="BM56" s="3"/>
     </row>
-    <row r="57" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -7174,7 +7175,7 @@
       <c r="BL57" s="3"/>
       <c r="BM57" s="3"/>
     </row>
-    <row r="58" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -7243,7 +7244,7 @@
       <c r="BL58" s="3"/>
       <c r="BM58" s="3"/>
     </row>
-    <row r="59" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -7312,7 +7313,7 @@
       <c r="BL59" s="3"/>
       <c r="BM59" s="3"/>
     </row>
-    <row r="60" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -7381,7 +7382,7 @@
       <c r="BL60" s="3"/>
       <c r="BM60" s="3"/>
     </row>
-    <row r="61" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -7450,7 +7451,7 @@
       <c r="BL61" s="3"/>
       <c r="BM61" s="3"/>
     </row>
-    <row r="62" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -7519,7 +7520,7 @@
       <c r="BL62" s="3"/>
       <c r="BM62" s="3"/>
     </row>
-    <row r="63" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -7588,7 +7589,7 @@
       <c r="BL63" s="3"/>
       <c r="BM63" s="3"/>
     </row>
-    <row r="64" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -7657,7 +7658,7 @@
       <c r="BL64" s="3"/>
       <c r="BM64" s="3"/>
     </row>
-    <row r="65" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -7726,7 +7727,7 @@
       <c r="BL65" s="3"/>
       <c r="BM65" s="3"/>
     </row>
-    <row r="66" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -7795,7 +7796,7 @@
       <c r="BL66" s="3"/>
       <c r="BM66" s="3"/>
     </row>
-    <row r="67" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -7864,7 +7865,7 @@
       <c r="BL67" s="3"/>
       <c r="BM67" s="3"/>
     </row>
-    <row r="68" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -7933,7 +7934,7 @@
       <c r="BL68" s="3"/>
       <c r="BM68" s="3"/>
     </row>
-    <row r="69" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -8002,7 +8003,7 @@
       <c r="BL69" s="3"/>
       <c r="BM69" s="3"/>
     </row>
-    <row r="70" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -8071,7 +8072,7 @@
       <c r="BL70" s="3"/>
       <c r="BM70" s="3"/>
     </row>
-    <row r="71" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -8140,7 +8141,7 @@
       <c r="BL71" s="3"/>
       <c r="BM71" s="3"/>
     </row>
-    <row r="72" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -8209,7 +8210,7 @@
       <c r="BL72" s="3"/>
       <c r="BM72" s="3"/>
     </row>
-    <row r="73" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -8278,7 +8279,7 @@
       <c r="BL73" s="3"/>
       <c r="BM73" s="3"/>
     </row>
-    <row r="74" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -8347,11 +8348,11 @@
       <c r="BL74" s="3"/>
       <c r="BM74" s="3"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D142" s="8"/>
       <c r="E142" s="8"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="8"/>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
@@ -8365,6 +8366,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="AQ2:AV2"/>
+    <mergeCell ref="AW2:BC2"/>
+    <mergeCell ref="BD2:BH2"/>
+    <mergeCell ref="BI2:BL2"/>
+    <mergeCell ref="BB3:BC3"/>
+    <mergeCell ref="AQ1:BM1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I1:AN1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="AO1:AP1"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="N5:O5"/>
@@ -8381,23 +8399,6 @@
     <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="AE3:AI3"/>
     <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AQ1:BM1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I1:AN1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="BG3:BH3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="AQ2:AV2"/>
-    <mergeCell ref="AW2:BC2"/>
-    <mergeCell ref="BD2:BH2"/>
-    <mergeCell ref="BI2:BL2"/>
-    <mergeCell ref="BB3:BC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -8412,21 +8413,21 @@
       <selection activeCell="J23" sqref="A23:J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="9" customWidth="1"/>
-    <col min="5" max="6" width="9.109375" style="9"/>
-    <col min="7" max="7" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="9" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="9"/>
+    <col min="7" max="7" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="7"/>
+    <col min="11" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>80</v>
       </c>
@@ -8448,7 +8449,7 @@
       </c>
       <c r="J1" s="32"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8480,7 +8481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>40</v>
       </c>
@@ -8520,7 +8521,7 @@
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>5</v>
@@ -8543,7 +8544,7 @@
       </c>
       <c r="R4" s="9"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>10</v>
@@ -8565,7 +8566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>15</v>
@@ -8587,7 +8588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>20</v>
@@ -8609,7 +8610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>25</v>
@@ -8631,7 +8632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>30</v>
@@ -8653,7 +8654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>35</v>
@@ -8675,7 +8676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>40</v>
@@ -8697,7 +8698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>45</v>
@@ -8719,7 +8720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>50</v>
@@ -8741,7 +8742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>55</v>
@@ -8764,7 +8765,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>60</v>
@@ -8791,7 +8792,7 @@
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>65</v>
@@ -8813,7 +8814,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>70</v>
@@ -8835,7 +8836,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>75</v>
@@ -8857,7 +8858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>80</v>
@@ -8890,7 +8891,7 @@
       <c r="T19" s="14"/>
       <c r="U19" s="14"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>85</v>
@@ -8910,7 +8911,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>90</v>
@@ -8930,7 +8931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>95</v>
@@ -8950,7 +8951,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -8966,55 +8967,55 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="14"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="14"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="14"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="14"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="14"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="14"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="14"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="14"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="14"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="14"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="14"/>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="14"/>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="14"/>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="14"/>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="14"/>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="14"/>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="14"/>
     </row>
   </sheetData>
@@ -9034,24 +9035,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C609DAD-BC63-4626-ACCC-69F8C32CB7AB}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A73" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="7"/>
+    <col min="1" max="1" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="31"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="29"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -9059,756 +9060,756 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="18" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="18" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="18" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="18" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="18" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="18" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="18" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="18" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="18" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="18" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="18" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="18" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="18" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="18" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="18" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="18" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="18" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="18" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="18" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="18" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="18" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="18" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="16"/>
       <c r="B103" s="18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="16"/>
       <c r="B104" s="18" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="16"/>
       <c r="B105" s="18" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="16"/>
       <c r="B106" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="16"/>
       <c r="B107" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="16"/>
       <c r="B108" s="18" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="16"/>
       <c r="B109" s="18" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="16"/>
       <c r="B110" s="18" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="16"/>
       <c r="B111" s="18" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="16"/>
       <c r="B112" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="16"/>
       <c r="B113" s="18" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="16"/>
       <c r="B114" s="18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="16"/>
       <c r="B115" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="16"/>
       <c r="B116" s="18" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="16"/>
       <c r="B117" s="18" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="16"/>
       <c r="B118" s="18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="16"/>
       <c r="B119" s="18" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="16"/>
       <c r="B120" s="18" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="16"/>
       <c r="B121" s="18" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="16"/>
       <c r="B122" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="16"/>
       <c r="B123" s="18" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="16"/>
       <c r="B124" s="18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="16"/>
       <c r="B125" s="18" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="16"/>
       <c r="B126" s="18" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="16"/>
       <c r="B127" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -9824,28 +9825,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84235012-AF5A-4BF0-8557-E62F3FAF9D19}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="7"/>
+    <col min="1" max="1" width="43.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
-        <v>225</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -9853,17 +9854,17 @@
         <v>2</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D2" s="35"/>
       <c r="E2" s="34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F2" s="35"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>91</v>
@@ -9881,7 +9882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="15" t="s">
         <v>92</v>
@@ -9899,7 +9900,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="15" t="s">
         <v>93</v>
@@ -9913,7 +9914,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="15" t="s">
         <v>94</v>
@@ -9927,10 +9928,10 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="15" t="s">
-        <v>95</v>
+        <v>231</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="20">
@@ -9941,10 +9942,10 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="20">
@@ -9955,10 +9956,10 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="20">
@@ -9969,40 +9970,40 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -10028,21 +10029,21 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="7"/>
+    <col min="1" max="1" width="19.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>87</v>
       </c>
       <c r="B1" s="26"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -10050,7 +10051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -10058,7 +10059,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>89</v>
@@ -10080,20 +10081,20 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="9"/>
-    <col min="3" max="16384" width="9.109375" style="7"/>
+    <col min="1" max="1" width="11.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="9"/>
+    <col min="3" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="26"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -10101,7 +10102,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>50</v>
       </c>
@@ -10109,115 +10110,115 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3">
         <v>100</v>

</xml_diff>

<commit_message>
1. Should be HVAC fix
</commit_message>
<xml_diff>
--- a/data/standards/InputJSONData.xlsx
+++ b/data/standards/InputJSONData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajszi\Documents\openstudio-standards\data\standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E9685D-130A-4F3E-886E-65799BD08870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD77681E-F251-4325-9966-1F4EB2B2F5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="5" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
   </bookViews>
@@ -715,9 +715,6 @@
     <t>IP</t>
   </si>
   <si>
-    <t>Ideal Air Loads with Ventilation</t>
-  </si>
-  <si>
     <t>Office-Conference</t>
   </si>
   <si>
@@ -728,6 +725,9 @@
   </si>
   <si>
     <t>PSZ-HP with Electric Auxiliary Heating</t>
+  </si>
+  <si>
+    <t>Ideal Loads with Ventilation</t>
   </si>
 </sst>
 </file>
@@ -943,6 +943,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -950,12 +956,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2396,74 +2396,74 @@
         <v>28</v>
       </c>
       <c r="E1" s="26"/>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="27" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="29"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="31"/>
       <c r="AO1" s="26" t="s">
         <v>32</v>
       </c>
       <c r="AP1" s="26"/>
-      <c r="AQ1" s="30" t="s">
+      <c r="AQ1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="30"/>
-      <c r="AS1" s="30"/>
-      <c r="AT1" s="30"/>
-      <c r="AU1" s="30"/>
-      <c r="AV1" s="30"/>
-      <c r="AW1" s="30"/>
-      <c r="AX1" s="30"/>
-      <c r="AY1" s="30"/>
-      <c r="AZ1" s="30"/>
-      <c r="BA1" s="30"/>
-      <c r="BB1" s="30"/>
-      <c r="BC1" s="30"/>
-      <c r="BD1" s="30"/>
-      <c r="BE1" s="30"/>
-      <c r="BF1" s="30"/>
-      <c r="BG1" s="30"/>
-      <c r="BH1" s="30"/>
-      <c r="BI1" s="30"/>
-      <c r="BJ1" s="30"/>
-      <c r="BK1" s="30"/>
-      <c r="BL1" s="30"/>
-      <c r="BM1" s="30"/>
+      <c r="AR1" s="28"/>
+      <c r="AS1" s="28"/>
+      <c r="AT1" s="28"/>
+      <c r="AU1" s="28"/>
+      <c r="AV1" s="28"/>
+      <c r="AW1" s="28"/>
+      <c r="AX1" s="28"/>
+      <c r="AY1" s="28"/>
+      <c r="AZ1" s="28"/>
+      <c r="BA1" s="28"/>
+      <c r="BB1" s="28"/>
+      <c r="BC1" s="28"/>
+      <c r="BD1" s="28"/>
+      <c r="BE1" s="28"/>
+      <c r="BF1" s="28"/>
+      <c r="BG1" s="28"/>
+      <c r="BH1" s="28"/>
+      <c r="BI1" s="28"/>
+      <c r="BJ1" s="28"/>
+      <c r="BK1" s="28"/>
+      <c r="BL1" s="28"/>
+      <c r="BM1" s="28"/>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2597,48 +2597,48 @@
       <c r="J3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="27" t="s">
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="27" t="s">
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="27" t="s">
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="AA3" s="28"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="28"/>
-      <c r="AD3" s="29"/>
-      <c r="AE3" s="27" t="s">
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="30"/>
+      <c r="AD3" s="31"/>
+      <c r="AE3" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="AF3" s="28"/>
-      <c r="AG3" s="28"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="29"/>
-      <c r="AJ3" s="27" t="s">
+      <c r="AF3" s="30"/>
+      <c r="AG3" s="30"/>
+      <c r="AH3" s="30"/>
+      <c r="AI3" s="31"/>
+      <c r="AJ3" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="28"/>
-      <c r="AM3" s="28"/>
-      <c r="AN3" s="29"/>
+      <c r="AK3" s="30"/>
+      <c r="AL3" s="30"/>
+      <c r="AM3" s="30"/>
+      <c r="AN3" s="31"/>
       <c r="AO3" s="3">
         <v>0</v>
       </c>
@@ -2678,10 +2678,10 @@
       <c r="BA3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="BB3" s="31" t="s">
+      <c r="BB3" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="BC3" s="31"/>
+      <c r="BC3" s="27"/>
       <c r="BD3" s="10" t="s">
         <v>57</v>
       </c>
@@ -2691,20 +2691,20 @@
       <c r="BF3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BG3" s="31" t="s">
+      <c r="BG3" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="BH3" s="31"/>
+      <c r="BH3" s="27"/>
       <c r="BI3" s="10" t="s">
         <v>57</v>
       </c>
       <c r="BJ3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BK3" s="31" t="s">
+      <c r="BK3" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="BL3" s="31"/>
+      <c r="BL3" s="27"/>
       <c r="BM3" s="10" t="s">
         <v>1</v>
       </c>
@@ -2735,57 +2735,57 @@
       <c r="K4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="29"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="31"/>
       <c r="P4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="27" t="s">
+      <c r="Q4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="29"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="31"/>
       <c r="U4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="27" t="s">
+      <c r="V4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="28"/>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="29"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="31"/>
       <c r="Z4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AA4" s="27" t="s">
+      <c r="AA4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="29"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="31"/>
       <c r="AE4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AF4" s="27" t="s">
+      <c r="AF4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AG4" s="28"/>
-      <c r="AH4" s="28"/>
-      <c r="AI4" s="29"/>
+      <c r="AG4" s="30"/>
+      <c r="AH4" s="30"/>
+      <c r="AI4" s="31"/>
       <c r="AJ4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AK4" s="27" t="s">
+      <c r="AK4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AL4" s="28"/>
-      <c r="AM4" s="28"/>
-      <c r="AN4" s="29"/>
+      <c r="AL4" s="30"/>
+      <c r="AM4" s="30"/>
+      <c r="AN4" s="31"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3">
         <v>5</v>
@@ -8366,23 +8366,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="BG3:BH3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="AQ2:AV2"/>
-    <mergeCell ref="AW2:BC2"/>
-    <mergeCell ref="BD2:BH2"/>
-    <mergeCell ref="BI2:BL2"/>
-    <mergeCell ref="BB3:BC3"/>
-    <mergeCell ref="AQ1:BM1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I1:AN1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="AO1:AP1"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="N5:O5"/>
@@ -8399,6 +8382,23 @@
     <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="AE3:AI3"/>
     <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AQ1:BM1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I1:AN1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="AQ2:AV2"/>
+    <mergeCell ref="AW2:BC2"/>
+    <mergeCell ref="BD2:BH2"/>
+    <mergeCell ref="BI2:BL2"/>
+    <mergeCell ref="BB3:BC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -9047,10 +9047,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -9095,7 +9095,7 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -9305,7 +9305,7 @@
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -9383,7 +9383,7 @@
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -9826,7 +9826,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9837,14 +9837,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -9931,7 +9931,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="20">
@@ -10003,7 +10003,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="16" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>

</xml_diff>

<commit_message>
1. College and Lab should be listed as Primary Building Type
</commit_message>
<xml_diff>
--- a/data/standards/InputJSONData.xlsx
+++ b/data/standards/InputJSONData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajszi\Documents\openstudio-standards\data\standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD14F5B7-D88E-4E8D-8465-5C72AF0F0862}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2679F97D-F0F2-493D-ADB5-A0D52B9A9DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="4" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectInformation" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="253">
   <si>
     <t>Primary_Building_Type</t>
   </si>
@@ -785,6 +785,12 @@
   </si>
   <si>
     <t>Lab-Open</t>
+  </si>
+  <si>
+    <t>College</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
   </si>
 </sst>
 </file>
@@ -933,7 +939,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1002,7 +1008,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1012,12 +1025,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1032,7 +1039,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1352,29 +1359,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB7C557-225C-4221-ACEB-8B371FDF63E0}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="D1" s="26"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1501,9 +1508,19 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -1512,6 +1529,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1546,10 +1564,10 @@
       <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="26"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2451,82 +2469,82 @@
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="27" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="27" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="29"/>
-      <c r="AO1" s="26" t="s">
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="AP1" s="26"/>
-      <c r="AQ1" s="30" t="s">
+      <c r="AP1" s="27"/>
+      <c r="AQ1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="30"/>
-      <c r="AS1" s="30"/>
-      <c r="AT1" s="30"/>
-      <c r="AU1" s="30"/>
-      <c r="AV1" s="30"/>
-      <c r="AW1" s="30"/>
-      <c r="AX1" s="30"/>
-      <c r="AY1" s="30"/>
-      <c r="AZ1" s="30"/>
-      <c r="BA1" s="30"/>
-      <c r="BB1" s="30"/>
-      <c r="BC1" s="30"/>
-      <c r="BD1" s="30"/>
-      <c r="BE1" s="30"/>
-      <c r="BF1" s="30"/>
-      <c r="BG1" s="30"/>
-      <c r="BH1" s="30"/>
-      <c r="BI1" s="30"/>
-      <c r="BJ1" s="30"/>
-      <c r="BK1" s="30"/>
-      <c r="BL1" s="30"/>
-      <c r="BM1" s="30"/>
+      <c r="AR1" s="29"/>
+      <c r="AS1" s="29"/>
+      <c r="AT1" s="29"/>
+      <c r="AU1" s="29"/>
+      <c r="AV1" s="29"/>
+      <c r="AW1" s="29"/>
+      <c r="AX1" s="29"/>
+      <c r="AY1" s="29"/>
+      <c r="AZ1" s="29"/>
+      <c r="BA1" s="29"/>
+      <c r="BB1" s="29"/>
+      <c r="BC1" s="29"/>
+      <c r="BD1" s="29"/>
+      <c r="BE1" s="29"/>
+      <c r="BF1" s="29"/>
+      <c r="BG1" s="29"/>
+      <c r="BH1" s="29"/>
+      <c r="BI1" s="29"/>
+      <c r="BJ1" s="29"/>
+      <c r="BK1" s="29"/>
+      <c r="BL1" s="29"/>
+      <c r="BM1" s="29"/>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2544,10 +2562,10 @@
       <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="26"/>
+      <c r="G2" s="27"/>
       <c r="H2" s="25" t="s">
         <v>224</v>
       </c>
@@ -2557,74 +2575,74 @@
       <c r="J2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="26"/>
-      <c r="AG2" s="26"/>
-      <c r="AH2" s="26"/>
-      <c r="AI2" s="26"/>
-      <c r="AJ2" s="26"/>
-      <c r="AK2" s="26"/>
-      <c r="AL2" s="26"/>
-      <c r="AM2" s="26"/>
-      <c r="AN2" s="26"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
+      <c r="AI2" s="27"/>
+      <c r="AJ2" s="27"/>
+      <c r="AK2" s="27"/>
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
       <c r="AO2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AP2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AQ2" s="26" t="s">
+      <c r="AQ2" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="AR2" s="26"/>
-      <c r="AS2" s="26"/>
-      <c r="AT2" s="26"/>
-      <c r="AU2" s="26"/>
-      <c r="AV2" s="26"/>
-      <c r="AW2" s="26" t="s">
+      <c r="AR2" s="27"/>
+      <c r="AS2" s="27"/>
+      <c r="AT2" s="27"/>
+      <c r="AU2" s="27"/>
+      <c r="AV2" s="27"/>
+      <c r="AW2" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="AX2" s="26"/>
-      <c r="AY2" s="26"/>
-      <c r="AZ2" s="26"/>
-      <c r="BA2" s="26"/>
-      <c r="BB2" s="26"/>
-      <c r="BC2" s="26"/>
-      <c r="BD2" s="26" t="s">
+      <c r="AX2" s="27"/>
+      <c r="AY2" s="27"/>
+      <c r="AZ2" s="27"/>
+      <c r="BA2" s="27"/>
+      <c r="BB2" s="27"/>
+      <c r="BC2" s="27"/>
+      <c r="BD2" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="BE2" s="26"/>
-      <c r="BF2" s="26"/>
-      <c r="BG2" s="26"/>
-      <c r="BH2" s="26"/>
-      <c r="BI2" s="26" t="s">
+      <c r="BE2" s="27"/>
+      <c r="BF2" s="27"/>
+      <c r="BG2" s="27"/>
+      <c r="BH2" s="27"/>
+      <c r="BI2" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="BJ2" s="26"/>
-      <c r="BK2" s="26"/>
-      <c r="BL2" s="26"/>
+      <c r="BJ2" s="27"/>
+      <c r="BK2" s="27"/>
+      <c r="BL2" s="27"/>
       <c r="BM2" s="5" t="s">
         <v>47</v>
       </c>
@@ -2660,48 +2678,48 @@
       <c r="J3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="27" t="s">
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="27" t="s">
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="27" t="s">
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="AA3" s="28"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="28"/>
-      <c r="AD3" s="29"/>
-      <c r="AE3" s="27" t="s">
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="31"/>
+      <c r="AD3" s="32"/>
+      <c r="AE3" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="AF3" s="28"/>
-      <c r="AG3" s="28"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="29"/>
-      <c r="AJ3" s="27" t="s">
+      <c r="AF3" s="31"/>
+      <c r="AG3" s="31"/>
+      <c r="AH3" s="31"/>
+      <c r="AI3" s="32"/>
+      <c r="AJ3" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="28"/>
-      <c r="AM3" s="28"/>
-      <c r="AN3" s="29"/>
+      <c r="AK3" s="31"/>
+      <c r="AL3" s="31"/>
+      <c r="AM3" s="31"/>
+      <c r="AN3" s="32"/>
       <c r="AO3" s="3">
         <v>0</v>
       </c>
@@ -2741,10 +2759,10 @@
       <c r="BA3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="BB3" s="31" t="s">
+      <c r="BB3" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="BC3" s="31"/>
+      <c r="BC3" s="28"/>
       <c r="BD3" s="10" t="s">
         <v>57</v>
       </c>
@@ -2754,20 +2772,20 @@
       <c r="BF3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BG3" s="31" t="s">
+      <c r="BG3" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="BH3" s="31"/>
+      <c r="BH3" s="28"/>
       <c r="BI3" s="10" t="s">
         <v>57</v>
       </c>
       <c r="BJ3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BK3" s="31" t="s">
+      <c r="BK3" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="BL3" s="31"/>
+      <c r="BL3" s="28"/>
       <c r="BM3" s="10" t="s">
         <v>1</v>
       </c>
@@ -2798,57 +2816,57 @@
       <c r="K4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="29"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="32"/>
       <c r="P4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="27" t="s">
+      <c r="Q4" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="29"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="32"/>
       <c r="U4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="27" t="s">
+      <c r="V4" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="28"/>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="29"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="32"/>
       <c r="Z4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AA4" s="27" t="s">
+      <c r="AA4" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="29"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="31"/>
+      <c r="AD4" s="32"/>
       <c r="AE4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AF4" s="27" t="s">
+      <c r="AF4" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="AG4" s="28"/>
-      <c r="AH4" s="28"/>
-      <c r="AI4" s="29"/>
+      <c r="AG4" s="31"/>
+      <c r="AH4" s="31"/>
+      <c r="AI4" s="32"/>
       <c r="AJ4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AK4" s="27" t="s">
+      <c r="AK4" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="AL4" s="28"/>
-      <c r="AM4" s="28"/>
-      <c r="AN4" s="29"/>
+      <c r="AL4" s="31"/>
+      <c r="AM4" s="31"/>
+      <c r="AN4" s="32"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3">
         <v>5</v>
@@ -2951,10 +2969,10 @@
       <c r="M5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="26" t="s">
+      <c r="N5" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="26"/>
+      <c r="O5" s="27"/>
       <c r="P5" s="3">
         <v>7</v>
       </c>
@@ -2964,10 +2982,10 @@
       <c r="R5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="S5" s="26" t="s">
+      <c r="S5" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="T5" s="26"/>
+      <c r="T5" s="27"/>
       <c r="U5" s="3">
         <v>13</v>
       </c>
@@ -2977,10 +2995,10 @@
       <c r="W5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="X5" s="26" t="s">
+      <c r="X5" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="Y5" s="26"/>
+      <c r="Y5" s="27"/>
       <c r="Z5" s="3">
         <v>9</v>
       </c>
@@ -2990,10 +3008,10 @@
       <c r="AB5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AC5" s="26" t="s">
+      <c r="AC5" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="AD5" s="26"/>
+      <c r="AD5" s="27"/>
       <c r="AE5" s="3">
         <v>13</v>
       </c>
@@ -3003,10 +3021,10 @@
       <c r="AG5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AH5" s="26" t="s">
+      <c r="AH5" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="AI5" s="26"/>
+      <c r="AI5" s="27"/>
       <c r="AJ5" s="3">
         <v>9</v>
       </c>
@@ -3016,10 +3034,10 @@
       <c r="AL5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AM5" s="26" t="s">
+      <c r="AM5" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="AN5" s="26"/>
+      <c r="AN5" s="27"/>
       <c r="AO5" s="3"/>
       <c r="AP5" s="3">
         <v>10</v>
@@ -8429,23 +8447,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="BG3:BH3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="AQ2:AV2"/>
-    <mergeCell ref="AW2:BC2"/>
-    <mergeCell ref="BD2:BH2"/>
-    <mergeCell ref="BI2:BL2"/>
-    <mergeCell ref="BB3:BC3"/>
-    <mergeCell ref="AQ1:BM1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I1:AN1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="AO1:AP1"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="N5:O5"/>
@@ -8462,6 +8463,23 @@
     <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="AE3:AI3"/>
     <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AQ1:BM1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I1:AN1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="AQ2:AV2"/>
+    <mergeCell ref="AW2:BC2"/>
+    <mergeCell ref="BD2:BH2"/>
+    <mergeCell ref="BI2:BL2"/>
+    <mergeCell ref="BB3:BC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -8491,26 +8509,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26" t="s">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="33" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32" t="s">
+      <c r="H1" s="33"/>
+      <c r="I1" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="32"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -9098,8 +9116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C609DAD-BC63-4626-ACCC-69F8C32CB7AB}">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B148" sqref="A146:B148"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9110,10 +9128,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -9877,127 +9895,127 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="16"/>
-      <c r="B128" s="36" t="s">
+      <c r="B128" s="26" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="16"/>
-      <c r="B129" s="36" t="s">
+      <c r="B129" s="26" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="16"/>
-      <c r="B130" s="36" t="s">
+      <c r="B130" s="26" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="16"/>
-      <c r="B131" s="36" t="s">
+      <c r="B131" s="26" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="16"/>
-      <c r="B132" s="36" t="s">
+      <c r="B132" s="26" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="16"/>
-      <c r="B133" s="36" t="s">
+      <c r="B133" s="26" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="16"/>
-      <c r="B134" s="36" t="s">
+      <c r="B134" s="26" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="16"/>
-      <c r="B135" s="36" t="s">
+      <c r="B135" s="26" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="16"/>
-      <c r="B136" s="36" t="s">
+      <c r="B136" s="26" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="16"/>
-      <c r="B137" s="36" t="s">
+      <c r="B137" s="26" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="16"/>
-      <c r="B138" s="36" t="s">
+      <c r="B138" s="26" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="16"/>
-      <c r="B139" s="36" t="s">
+      <c r="B139" s="26" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="16"/>
-      <c r="B140" s="36" t="s">
+      <c r="B140" s="26" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="16"/>
-      <c r="B141" s="36" t="s">
+      <c r="B141" s="26" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="16"/>
-      <c r="B142" s="36" t="s">
+      <c r="B142" s="26" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="16"/>
-      <c r="B143" s="36" t="s">
+      <c r="B143" s="26" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="16"/>
-      <c r="B144" s="36" t="s">
+      <c r="B144" s="26" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="16"/>
-      <c r="B145" s="36" t="s">
+      <c r="B145" s="26" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="16"/>
-      <c r="B146" s="36" t="s">
+      <c r="B146" s="26" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="16"/>
-      <c r="B147" s="36" t="s">
+      <c r="B147" s="26" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="16"/>
-      <c r="B148" s="36" t="s">
+      <c r="B148" s="26" t="s">
         <v>250</v>
       </c>
     </row>
@@ -10026,14 +10044,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -10042,14 +10060,14 @@
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="34" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="F2" s="35"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -10227,10 +10245,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -10278,10 +10296,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">

</xml_diff>

<commit_message>
Revert "1. Adding college and lab export successful"
This reverts commit 59edd931ba764e19078b01b7498b0b1bfd74b571.
</commit_message>
<xml_diff>
--- a/data/standards/InputJSONData.xlsx
+++ b/data/standards/InputJSONData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajszi\Documents\openstudio-standards\data\standards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\pw-openstudio-standards\data\standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD14F5B7-D88E-4E8D-8465-5C72AF0F0862}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB54548-290B-4892-932C-14C45D77557D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="4" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="868" activeTab="4" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectInformation" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="232">
   <si>
     <t>Primary_Building_Type</t>
   </si>
@@ -728,63 +728,6 @@
   </si>
   <si>
     <t>Outpatient-Cafe</t>
-  </si>
-  <si>
-    <t>College-Conference</t>
-  </si>
-  <si>
-    <t>College-Corridor</t>
-  </si>
-  <si>
-    <t>College-ElevatorShaft</t>
-  </si>
-  <si>
-    <t>College-EnteranceLobby</t>
-  </si>
-  <si>
-    <t>College-Lounge</t>
-  </si>
-  <si>
-    <t>College-Office</t>
-  </si>
-  <si>
-    <t>College-Restroom</t>
-  </si>
-  <si>
-    <t>College-Utility</t>
-  </si>
-  <si>
-    <t>College-ArtClassroom</t>
-  </si>
-  <si>
-    <t>College-Classroom</t>
-  </si>
-  <si>
-    <t>College-Laboratory</t>
-  </si>
-  <si>
-    <t>College-LectureHall</t>
-  </si>
-  <si>
-    <t>College-MediaCenter</t>
-  </si>
-  <si>
-    <t>College-Stairs</t>
-  </si>
-  <si>
-    <t>College-Storage</t>
-  </si>
-  <si>
-    <t>Lab-Equipment_corridor</t>
-  </si>
-  <si>
-    <t>Lab-Lab_fumehood</t>
-  </si>
-  <si>
-    <t>Lab-Office</t>
-  </si>
-  <si>
-    <t>Lab-Open</t>
   </si>
 </sst>
 </file>
@@ -830,18 +773,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -933,7 +870,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1005,6 +942,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1012,12 +955,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1032,7 +969,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1358,15 +1294,15 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -1376,7 +1312,7 @@
       </c>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1390,7 +1326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1404,7 +1340,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="6" t="s">
         <v>24</v>
@@ -1412,7 +1348,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>25</v>
@@ -1420,7 +1356,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -1428,7 +1364,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -1436,7 +1372,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -1444,7 +1380,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -1452,55 +1388,55 @@
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
@@ -1523,14 +1459,14 @@
       <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="9.140625" style="9"/>
-    <col min="8" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="15.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9.109375" style="9"/>
+    <col min="8" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1551,7 +1487,7 @@
       </c>
       <c r="G1" s="26"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1574,7 +1510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>150</v>
       </c>
@@ -1597,7 +1533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1608,7 +1544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1619,7 +1555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1630,7 +1566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1641,7 +1577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1652,7 +1588,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1663,7 +1599,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1674,7 +1610,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1685,7 +1621,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1696,7 +1632,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1707,7 +1643,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1718,7 +1654,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1729,7 +1665,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1740,7 +1676,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1751,7 +1687,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1762,7 +1698,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1773,7 +1709,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1784,7 +1720,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1795,7 +1731,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1806,7 +1742,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1817,7 +1753,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1828,7 +1764,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1839,7 +1775,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1850,7 +1786,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1861,7 +1797,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1872,7 +1808,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1883,7 +1819,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1894,7 +1830,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1905,7 +1841,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1916,7 +1852,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1927,7 +1863,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1938,7 +1874,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1949,7 +1885,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1960,7 +1896,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1971,7 +1907,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1982,7 +1918,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1993,7 +1929,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -2004,7 +1940,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -2015,7 +1951,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -2026,7 +1962,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -2037,7 +1973,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -2048,7 +1984,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -2059,7 +1995,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2070,7 +2006,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2081,7 +2017,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -2092,7 +2028,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2103,7 +2039,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -2114,7 +2050,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -2125,7 +2061,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2136,7 +2072,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -2147,7 +2083,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -2158,7 +2094,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -2169,7 +2105,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -2180,7 +2116,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -2191,7 +2127,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -2202,7 +2138,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -2213,7 +2149,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -2224,7 +2160,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -2235,7 +2171,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -2246,7 +2182,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="5"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -2257,7 +2193,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -2268,7 +2204,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="5"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -2279,7 +2215,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -2290,7 +2226,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -2301,7 +2237,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -2312,7 +2248,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -2323,7 +2259,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -2334,7 +2270,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -2345,7 +2281,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -2356,7 +2292,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -2367,7 +2303,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -2395,59 +2331,59 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="36" max="38" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="39" max="40" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" style="9" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="38" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="66" max="16384" width="9.140625" style="9"/>
+    <col min="46" max="46" width="18.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="66" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
@@ -2459,76 +2395,76 @@
         <v>28</v>
       </c>
       <c r="E1" s="26"/>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="27" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="29"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="31"/>
       <c r="AO1" s="26" t="s">
         <v>32</v>
       </c>
       <c r="AP1" s="26"/>
-      <c r="AQ1" s="30" t="s">
+      <c r="AQ1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="30"/>
-      <c r="AS1" s="30"/>
-      <c r="AT1" s="30"/>
-      <c r="AU1" s="30"/>
-      <c r="AV1" s="30"/>
-      <c r="AW1" s="30"/>
-      <c r="AX1" s="30"/>
-      <c r="AY1" s="30"/>
-      <c r="AZ1" s="30"/>
-      <c r="BA1" s="30"/>
-      <c r="BB1" s="30"/>
-      <c r="BC1" s="30"/>
-      <c r="BD1" s="30"/>
-      <c r="BE1" s="30"/>
-      <c r="BF1" s="30"/>
-      <c r="BG1" s="30"/>
-      <c r="BH1" s="30"/>
-      <c r="BI1" s="30"/>
-      <c r="BJ1" s="30"/>
-      <c r="BK1" s="30"/>
-      <c r="BL1" s="30"/>
-      <c r="BM1" s="30"/>
-    </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="AR1" s="28"/>
+      <c r="AS1" s="28"/>
+      <c r="AT1" s="28"/>
+      <c r="AU1" s="28"/>
+      <c r="AV1" s="28"/>
+      <c r="AW1" s="28"/>
+      <c r="AX1" s="28"/>
+      <c r="AY1" s="28"/>
+      <c r="AZ1" s="28"/>
+      <c r="BA1" s="28"/>
+      <c r="BB1" s="28"/>
+      <c r="BC1" s="28"/>
+      <c r="BD1" s="28"/>
+      <c r="BE1" s="28"/>
+      <c r="BF1" s="28"/>
+      <c r="BG1" s="28"/>
+      <c r="BH1" s="28"/>
+      <c r="BI1" s="28"/>
+      <c r="BJ1" s="28"/>
+      <c r="BK1" s="28"/>
+      <c r="BL1" s="28"/>
+      <c r="BM1" s="28"/>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2629,7 +2565,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>200000</v>
       </c>
@@ -2660,48 +2596,48 @@
       <c r="J3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="27" t="s">
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="27" t="s">
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="27" t="s">
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="AA3" s="28"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="28"/>
-      <c r="AD3" s="29"/>
-      <c r="AE3" s="27" t="s">
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="30"/>
+      <c r="AD3" s="31"/>
+      <c r="AE3" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="AF3" s="28"/>
-      <c r="AG3" s="28"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="29"/>
-      <c r="AJ3" s="27" t="s">
+      <c r="AF3" s="30"/>
+      <c r="AG3" s="30"/>
+      <c r="AH3" s="30"/>
+      <c r="AI3" s="31"/>
+      <c r="AJ3" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="28"/>
-      <c r="AM3" s="28"/>
-      <c r="AN3" s="29"/>
+      <c r="AK3" s="30"/>
+      <c r="AL3" s="30"/>
+      <c r="AM3" s="30"/>
+      <c r="AN3" s="31"/>
       <c r="AO3" s="3">
         <v>0</v>
       </c>
@@ -2741,10 +2677,10 @@
       <c r="BA3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="BB3" s="31" t="s">
+      <c r="BB3" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="BC3" s="31"/>
+      <c r="BC3" s="27"/>
       <c r="BD3" s="10" t="s">
         <v>57</v>
       </c>
@@ -2754,25 +2690,25 @@
       <c r="BF3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BG3" s="31" t="s">
+      <c r="BG3" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="BH3" s="31"/>
+      <c r="BH3" s="27"/>
       <c r="BI3" s="10" t="s">
         <v>57</v>
       </c>
       <c r="BJ3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BK3" s="31" t="s">
+      <c r="BK3" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="BL3" s="31"/>
+      <c r="BL3" s="27"/>
       <c r="BM3" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
@@ -2798,57 +2734,57 @@
       <c r="K4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="29"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="31"/>
       <c r="P4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="27" t="s">
+      <c r="Q4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="29"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="31"/>
       <c r="U4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="27" t="s">
+      <c r="V4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="28"/>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="29"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="31"/>
       <c r="Z4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AA4" s="27" t="s">
+      <c r="AA4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="29"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="31"/>
       <c r="AE4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AF4" s="27" t="s">
+      <c r="AF4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AG4" s="28"/>
-      <c r="AH4" s="28"/>
-      <c r="AI4" s="29"/>
+      <c r="AG4" s="30"/>
+      <c r="AH4" s="30"/>
+      <c r="AI4" s="31"/>
       <c r="AJ4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AK4" s="27" t="s">
+      <c r="AK4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AL4" s="28"/>
-      <c r="AM4" s="28"/>
-      <c r="AN4" s="29"/>
+      <c r="AL4" s="30"/>
+      <c r="AM4" s="30"/>
+      <c r="AN4" s="31"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3">
         <v>5</v>
@@ -2923,7 +2859,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="5"/>
       <c r="C5" s="3">
@@ -3092,7 +3028,7 @@
       </c>
       <c r="BM5" s="10"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
@@ -3223,7 +3159,7 @@
       </c>
       <c r="BM6" s="10"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -3340,7 +3276,7 @@
       </c>
       <c r="BM7" s="10"/>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -3445,7 +3381,7 @@
       </c>
       <c r="BM8" s="10"/>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="3">
@@ -3548,7 +3484,7 @@
       </c>
       <c r="BM9" s="10"/>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -3645,7 +3581,7 @@
       <c r="BL10" s="3"/>
       <c r="BM10" s="3"/>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -3742,7 +3678,7 @@
       <c r="BL11" s="3"/>
       <c r="BM11" s="3"/>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="3">
@@ -3839,7 +3775,7 @@
       <c r="BL12" s="3"/>
       <c r="BM12" s="3"/>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -3936,7 +3872,7 @@
       <c r="BL13" s="3"/>
       <c r="BM13" s="3"/>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3">
@@ -4033,7 +3969,7 @@
       <c r="BL14" s="3"/>
       <c r="BM14" s="3"/>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
@@ -4130,7 +4066,7 @@
       <c r="BL15" s="3"/>
       <c r="BM15" s="3"/>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3">
@@ -4227,7 +4163,7 @@
       <c r="BL16" s="3"/>
       <c r="BM16" s="3"/>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
@@ -4324,7 +4260,7 @@
       <c r="BL17" s="3"/>
       <c r="BM17" s="3"/>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3">
@@ -4421,7 +4357,7 @@
       <c r="BL18" s="3"/>
       <c r="BM18" s="3"/>
     </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3">
@@ -4518,7 +4454,7 @@
       <c r="BL19" s="3"/>
       <c r="BM19" s="3"/>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3">
@@ -4591,7 +4527,7 @@
       <c r="BL20" s="3"/>
       <c r="BM20" s="3"/>
     </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3">
@@ -4664,7 +4600,7 @@
       <c r="BL21" s="3"/>
       <c r="BM21" s="3"/>
     </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3">
@@ -4737,7 +4673,7 @@
       <c r="BL22" s="3"/>
       <c r="BM22" s="3"/>
     </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3">
@@ -4810,7 +4746,7 @@
       <c r="BL23" s="3"/>
       <c r="BM23" s="3"/>
     </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3">
@@ -4883,7 +4819,7 @@
       <c r="BL24" s="3"/>
       <c r="BM24" s="3"/>
     </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3">
@@ -4956,7 +4892,7 @@
       <c r="BL25" s="3"/>
       <c r="BM25" s="3"/>
     </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3">
@@ -5029,7 +4965,7 @@
       <c r="BL26" s="3"/>
       <c r="BM26" s="3"/>
     </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3">
@@ -5102,7 +5038,7 @@
       <c r="BL27" s="3"/>
       <c r="BM27" s="3"/>
     </row>
-    <row r="28" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3">
@@ -5175,7 +5111,7 @@
       <c r="BL28" s="3"/>
       <c r="BM28" s="3"/>
     </row>
-    <row r="29" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3">
@@ -5248,7 +5184,7 @@
       <c r="BL29" s="3"/>
       <c r="BM29" s="3"/>
     </row>
-    <row r="30" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3">
@@ -5321,7 +5257,7 @@
       <c r="BL30" s="3"/>
       <c r="BM30" s="3"/>
     </row>
-    <row r="31" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3">
@@ -5394,7 +5330,7 @@
       <c r="BL31" s="3"/>
       <c r="BM31" s="3"/>
     </row>
-    <row r="32" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3">
@@ -5467,7 +5403,7 @@
       <c r="BL32" s="3"/>
       <c r="BM32" s="3"/>
     </row>
-    <row r="33" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3">
@@ -5540,7 +5476,7 @@
       <c r="BL33" s="3"/>
       <c r="BM33" s="3"/>
     </row>
-    <row r="34" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3">
@@ -5613,7 +5549,7 @@
       <c r="BL34" s="3"/>
       <c r="BM34" s="3"/>
     </row>
-    <row r="35" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3">
@@ -5686,7 +5622,7 @@
       <c r="BL35" s="3"/>
       <c r="BM35" s="3"/>
     </row>
-    <row r="36" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3">
@@ -5757,7 +5693,7 @@
       <c r="BL36" s="3"/>
       <c r="BM36" s="3"/>
     </row>
-    <row r="37" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3">
@@ -5828,7 +5764,7 @@
       <c r="BL37" s="3"/>
       <c r="BM37" s="3"/>
     </row>
-    <row r="38" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3">
@@ -5899,7 +5835,7 @@
       <c r="BL38" s="3"/>
       <c r="BM38" s="3"/>
     </row>
-    <row r="39" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3">
@@ -5970,7 +5906,7 @@
       <c r="BL39" s="3"/>
       <c r="BM39" s="3"/>
     </row>
-    <row r="40" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3">
@@ -6041,7 +5977,7 @@
       <c r="BL40" s="3"/>
       <c r="BM40" s="3"/>
     </row>
-    <row r="41" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3">
@@ -6112,7 +6048,7 @@
       <c r="BL41" s="3"/>
       <c r="BM41" s="3"/>
     </row>
-    <row r="42" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3">
@@ -6183,7 +6119,7 @@
       <c r="BL42" s="3"/>
       <c r="BM42" s="3"/>
     </row>
-    <row r="43" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3">
@@ -6254,7 +6190,7 @@
       <c r="BL43" s="3"/>
       <c r="BM43" s="3"/>
     </row>
-    <row r="44" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3">
@@ -6325,7 +6261,7 @@
       <c r="BL44" s="3"/>
       <c r="BM44" s="3"/>
     </row>
-    <row r="45" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3">
@@ -6396,7 +6332,7 @@
       <c r="BL45" s="3"/>
       <c r="BM45" s="3"/>
     </row>
-    <row r="46" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3">
@@ -6467,7 +6403,7 @@
       <c r="BL46" s="3"/>
       <c r="BM46" s="3"/>
     </row>
-    <row r="47" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3">
@@ -6538,7 +6474,7 @@
       <c r="BL47" s="3"/>
       <c r="BM47" s="3"/>
     </row>
-    <row r="48" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3">
@@ -6609,7 +6545,7 @@
       <c r="BL48" s="3"/>
       <c r="BM48" s="3"/>
     </row>
-    <row r="49" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3">
@@ -6680,7 +6616,7 @@
       <c r="BL49" s="3"/>
       <c r="BM49" s="3"/>
     </row>
-    <row r="50" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3">
@@ -6751,7 +6687,7 @@
       <c r="BL50" s="3"/>
       <c r="BM50" s="3"/>
     </row>
-    <row r="51" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3">
@@ -6822,7 +6758,7 @@
       <c r="BL51" s="3"/>
       <c r="BM51" s="3"/>
     </row>
-    <row r="52" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3">
@@ -6893,7 +6829,7 @@
       <c r="BL52" s="3"/>
       <c r="BM52" s="3"/>
     </row>
-    <row r="53" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -6962,7 +6898,7 @@
       <c r="BL53" s="3"/>
       <c r="BM53" s="3"/>
     </row>
-    <row r="54" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -7031,7 +6967,7 @@
       <c r="BL54" s="3"/>
       <c r="BM54" s="3"/>
     </row>
-    <row r="55" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -7100,7 +7036,7 @@
       <c r="BL55" s="3"/>
       <c r="BM55" s="3"/>
     </row>
-    <row r="56" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -7169,7 +7105,7 @@
       <c r="BL56" s="3"/>
       <c r="BM56" s="3"/>
     </row>
-    <row r="57" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -7238,7 +7174,7 @@
       <c r="BL57" s="3"/>
       <c r="BM57" s="3"/>
     </row>
-    <row r="58" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -7307,7 +7243,7 @@
       <c r="BL58" s="3"/>
       <c r="BM58" s="3"/>
     </row>
-    <row r="59" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -7376,7 +7312,7 @@
       <c r="BL59" s="3"/>
       <c r="BM59" s="3"/>
     </row>
-    <row r="60" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -7445,7 +7381,7 @@
       <c r="BL60" s="3"/>
       <c r="BM60" s="3"/>
     </row>
-    <row r="61" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -7514,7 +7450,7 @@
       <c r="BL61" s="3"/>
       <c r="BM61" s="3"/>
     </row>
-    <row r="62" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -7583,7 +7519,7 @@
       <c r="BL62" s="3"/>
       <c r="BM62" s="3"/>
     </row>
-    <row r="63" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -7652,7 +7588,7 @@
       <c r="BL63" s="3"/>
       <c r="BM63" s="3"/>
     </row>
-    <row r="64" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -7721,7 +7657,7 @@
       <c r="BL64" s="3"/>
       <c r="BM64" s="3"/>
     </row>
-    <row r="65" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -7790,7 +7726,7 @@
       <c r="BL65" s="3"/>
       <c r="BM65" s="3"/>
     </row>
-    <row r="66" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -7859,7 +7795,7 @@
       <c r="BL66" s="3"/>
       <c r="BM66" s="3"/>
     </row>
-    <row r="67" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -7928,7 +7864,7 @@
       <c r="BL67" s="3"/>
       <c r="BM67" s="3"/>
     </row>
-    <row r="68" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -7997,7 +7933,7 @@
       <c r="BL68" s="3"/>
       <c r="BM68" s="3"/>
     </row>
-    <row r="69" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -8066,7 +8002,7 @@
       <c r="BL69" s="3"/>
       <c r="BM69" s="3"/>
     </row>
-    <row r="70" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -8135,7 +8071,7 @@
       <c r="BL70" s="3"/>
       <c r="BM70" s="3"/>
     </row>
-    <row r="71" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -8204,7 +8140,7 @@
       <c r="BL71" s="3"/>
       <c r="BM71" s="3"/>
     </row>
-    <row r="72" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -8273,7 +8209,7 @@
       <c r="BL72" s="3"/>
       <c r="BM72" s="3"/>
     </row>
-    <row r="73" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -8342,7 +8278,7 @@
       <c r="BL73" s="3"/>
       <c r="BM73" s="3"/>
     </row>
-    <row r="74" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -8411,11 +8347,11 @@
       <c r="BL74" s="3"/>
       <c r="BM74" s="3"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D142" s="8"/>
       <c r="E142" s="8"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" s="8"/>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
@@ -8429,23 +8365,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="BG3:BH3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="AQ2:AV2"/>
-    <mergeCell ref="AW2:BC2"/>
-    <mergeCell ref="BD2:BH2"/>
-    <mergeCell ref="BI2:BL2"/>
-    <mergeCell ref="BB3:BC3"/>
-    <mergeCell ref="AQ1:BM1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I1:AN1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="AO1:AP1"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="N5:O5"/>
@@ -8462,6 +8381,23 @@
     <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="AE3:AI3"/>
     <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AQ1:BM1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I1:AN1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="AQ2:AV2"/>
+    <mergeCell ref="AW2:BC2"/>
+    <mergeCell ref="BD2:BH2"/>
+    <mergeCell ref="BI2:BL2"/>
+    <mergeCell ref="BB3:BC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -8476,21 +8412,21 @@
       <selection activeCell="J23" sqref="A23:J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="9" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="9"/>
-    <col min="7" max="7" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="9" customWidth="1"/>
+    <col min="5" max="6" width="9.109375" style="9"/>
+    <col min="7" max="7" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="7"/>
+    <col min="11" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>80</v>
       </c>
@@ -8512,7 +8448,7 @@
       </c>
       <c r="J1" s="32"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8544,7 +8480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>40</v>
       </c>
@@ -8584,7 +8520,7 @@
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>5</v>
@@ -8607,7 +8543,7 @@
       </c>
       <c r="R4" s="9"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>10</v>
@@ -8629,7 +8565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>15</v>
@@ -8651,7 +8587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>20</v>
@@ -8673,7 +8609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>25</v>
@@ -8695,7 +8631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>30</v>
@@ -8717,7 +8653,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>35</v>
@@ -8739,7 +8675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>40</v>
@@ -8761,7 +8697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>45</v>
@@ -8783,7 +8719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>50</v>
@@ -8805,7 +8741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>55</v>
@@ -8828,7 +8764,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>60</v>
@@ -8855,7 +8791,7 @@
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>65</v>
@@ -8877,7 +8813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>70</v>
@@ -8899,7 +8835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>75</v>
@@ -8921,7 +8857,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>80</v>
@@ -8954,7 +8890,7 @@
       <c r="T19" s="14"/>
       <c r="U19" s="14"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>85</v>
@@ -8974,7 +8910,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>90</v>
@@ -8994,7 +8930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>95</v>
@@ -9014,7 +8950,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -9030,55 +8966,55 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C47" s="14"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C48" s="14"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" s="14"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" s="14"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C51" s="14"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52" s="14"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53" s="14"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54" s="14"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55" s="14"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56" s="14"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" s="14"/>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C58" s="14"/>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" s="14"/>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C60" s="14"/>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" s="14"/>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C62" s="14"/>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C63" s="14"/>
     </row>
   </sheetData>
@@ -9096,26 +9032,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C609DAD-BC63-4626-ACCC-69F8C32CB7AB}">
-  <dimension ref="A1:B148"/>
+  <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B148" sqref="A146:B148"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="29"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="31"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -9123,7 +9059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -9131,874 +9067,748 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="18" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="18" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="18" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="18" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="18" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="18" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="18" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="18" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="18" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="18" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="18" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="18" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="18" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="18" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="18" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="18" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="18" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="18" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="18" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="18" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="18" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="18" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="18" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="18" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="18" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="18" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="18" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="18" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="18" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="18" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="18" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="18" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="18" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="18" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="18" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="18" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="18" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="18" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="18" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="18" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="18" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="18" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="18" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="18" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="18" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="18" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="18" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="18" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="18" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="18" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="18" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="18" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="18" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="18" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="18" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="4"/>
       <c r="B75" s="18" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="B76" s="18" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
       <c r="B77" s="18" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="B78" s="18" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="4"/>
       <c r="B79" s="18" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="4"/>
       <c r="B80" s="18" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="4"/>
       <c r="B81" s="18" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="B82" s="18" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="4"/>
       <c r="B83" s="18" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
       <c r="B84" s="18" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="4"/>
       <c r="B85" s="18" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="4"/>
       <c r="B86" s="18" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="4"/>
       <c r="B87" s="18" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="4"/>
       <c r="B88" s="18" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="4"/>
       <c r="B89" s="18" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="4"/>
       <c r="B90" s="18" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="4"/>
       <c r="B91" s="18" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="4"/>
       <c r="B92" s="18" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="4"/>
       <c r="B93" s="18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="4"/>
       <c r="B94" s="18" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="4"/>
       <c r="B95" s="18" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="4"/>
       <c r="B96" s="18" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="4"/>
       <c r="B97" s="18" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="4"/>
       <c r="B98" s="18" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="4"/>
       <c r="B99" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="4"/>
       <c r="B100" s="18" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="4"/>
       <c r="B101" s="18" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="4"/>
       <c r="B102" s="18" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="16"/>
       <c r="B103" s="18" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="16"/>
       <c r="B104" s="18" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="16"/>
       <c r="B105" s="18" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="16"/>
       <c r="B106" s="18" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="16"/>
       <c r="B107" s="18" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="16"/>
       <c r="B108" s="18" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="16"/>
       <c r="B109" s="18" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="16"/>
       <c r="B110" s="18" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="16"/>
       <c r="B111" s="18" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="16"/>
       <c r="B112" s="18" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="16"/>
       <c r="B113" s="18" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="16"/>
       <c r="B114" s="18" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="16"/>
       <c r="B115" s="18" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="16"/>
       <c r="B116" s="18" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="16"/>
       <c r="B117" s="18" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="16"/>
       <c r="B118" s="18" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="16"/>
       <c r="B119" s="18" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="16"/>
       <c r="B120" s="18" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="16"/>
       <c r="B121" s="18" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="16"/>
       <c r="B122" s="18" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="16"/>
       <c r="B123" s="18" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="16"/>
       <c r="B124" s="18" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="16"/>
       <c r="B125" s="18" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="16"/>
       <c r="B126" s="18" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="16"/>
       <c r="B127" s="18" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="16"/>
-      <c r="B128" s="36" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="16"/>
-      <c r="B129" s="36" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="16"/>
-      <c r="B130" s="36" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="16"/>
-      <c r="B131" s="36" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="16"/>
-      <c r="B132" s="36" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="16"/>
-      <c r="B133" s="36" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="16"/>
-      <c r="B134" s="36" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="16"/>
-      <c r="B135" s="36" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="16"/>
-      <c r="B136" s="36" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="16"/>
-      <c r="B137" s="36" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="16"/>
-      <c r="B138" s="36" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="16"/>
-      <c r="B139" s="36" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="16"/>
-      <c r="B140" s="36" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="16"/>
-      <c r="B141" s="36" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="16"/>
-      <c r="B142" s="36" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="16"/>
-      <c r="B143" s="36" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="16"/>
-      <c r="B144" s="36" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="16"/>
-      <c r="B145" s="36" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="16"/>
-      <c r="B146" s="36" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="16"/>
-      <c r="B147" s="36" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="16"/>
-      <c r="B148" s="36" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -10018,24 +9828,24 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="43.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -10051,7 +9861,7 @@
       </c>
       <c r="F2" s="35"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>98</v>
       </c>
@@ -10071,7 +9881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="15" t="s">
         <v>92</v>
@@ -10089,7 +9899,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="15" t="s">
         <v>93</v>
@@ -10103,7 +9913,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="15" t="s">
         <v>94</v>
@@ -10117,7 +9927,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="15" t="s">
         <v>95</v>
@@ -10131,7 +9941,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="15" t="s">
         <v>96</v>
@@ -10145,7 +9955,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="15" t="s">
         <v>97</v>
@@ -10159,7 +9969,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="15" t="s">
         <v>98</v>
@@ -10169,7 +9979,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="15" t="s">
         <v>99</v>
@@ -10179,7 +9989,7 @@
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="15" t="s">
         <v>100</v>
@@ -10189,7 +9999,7 @@
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="16" t="s">
         <v>228</v>
@@ -10218,21 +10028,21 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="19.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>87</v>
       </c>
       <c r="B1" s="26"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -10240,7 +10050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -10248,7 +10058,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>89</v>
@@ -10270,20 +10080,20 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="9"/>
-    <col min="3" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="11.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="9"/>
+    <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="26"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -10291,7 +10101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>50</v>
       </c>
@@ -10299,115 +10109,115 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3">
         <v>100</v>

</xml_diff>

<commit_message>
1. Fix for incorrect hvac names PSZ-HP with Gas Auxiliary Heating to PSZ-HP with Electric Auxiliary Heating Ideal Loads with Ventilation for ideal loads
</commit_message>
<xml_diff>
--- a/data/standards/InputJSONData.xlsx
+++ b/data/standards/InputJSONData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajszi\Documents\openstudio-standards\data\standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2679F97D-F0F2-493D-ADB5-A0D52B9A9DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3EFA9B-C04D-4A95-8FE0-F935D5E389F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="5" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectInformation" sheetId="1" r:id="rId1"/>
@@ -319,9 +319,6 @@
     <t>PSZ-AC with Gas Heating</t>
   </si>
   <si>
-    <t>PSZ-HP with Gas Auxiliary Heating</t>
-  </si>
-  <si>
     <t>Fan Coils with Water-Cooled Chiller and Boiler HW Heating</t>
   </si>
   <si>
@@ -718,9 +715,6 @@
     <t>IP</t>
   </si>
   <si>
-    <t>Ideal Air Loads with Ventilation</t>
-  </si>
-  <si>
     <t>Office-Conference</t>
   </si>
   <si>
@@ -791,6 +785,12 @@
   </si>
   <si>
     <t>Laboratory</t>
+  </si>
+  <si>
+    <t>PSZ-HP with Electric Auxiliary Heating</t>
+  </si>
+  <si>
+    <t>Ideal Loads with Ventilation</t>
   </si>
 </sst>
 </file>
@@ -1009,13 +1009,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1025,6 +1020,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1039,7 +1040,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1361,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB7C557-225C-4221-ACEB-8B371FDF63E0}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,14 +1374,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1405,10 +1405,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1508,19 +1508,19 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -1564,10 +1564,10 @@
       <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="27"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2469,82 +2469,82 @@
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="30" t="s">
+      <c r="E1" s="28"/>
+      <c r="F1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="30" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="27" t="s">
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="29" t="s">
+      <c r="AP1" s="28"/>
+      <c r="AQ1" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="29"/>
-      <c r="AS1" s="29"/>
-      <c r="AT1" s="29"/>
-      <c r="AU1" s="29"/>
-      <c r="AV1" s="29"/>
-      <c r="AW1" s="29"/>
-      <c r="AX1" s="29"/>
-      <c r="AY1" s="29"/>
-      <c r="AZ1" s="29"/>
-      <c r="BA1" s="29"/>
-      <c r="BB1" s="29"/>
-      <c r="BC1" s="29"/>
-      <c r="BD1" s="29"/>
-      <c r="BE1" s="29"/>
-      <c r="BF1" s="29"/>
-      <c r="BG1" s="29"/>
-      <c r="BH1" s="29"/>
-      <c r="BI1" s="29"/>
-      <c r="BJ1" s="29"/>
-      <c r="BK1" s="29"/>
-      <c r="BL1" s="29"/>
-      <c r="BM1" s="29"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2562,12 +2562,12 @@
       <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="27"/>
+      <c r="G2" s="28"/>
       <c r="H2" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>1</v>
@@ -2575,74 +2575,74 @@
       <c r="J2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="27"/>
-      <c r="AG2" s="27"/>
-      <c r="AH2" s="27"/>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="27"/>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28"/>
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="28"/>
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
       <c r="AO2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AP2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AQ2" s="27" t="s">
+      <c r="AQ2" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="AR2" s="27"/>
-      <c r="AS2" s="27"/>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
-      <c r="AW2" s="27" t="s">
+      <c r="AR2" s="28"/>
+      <c r="AS2" s="28"/>
+      <c r="AT2" s="28"/>
+      <c r="AU2" s="28"/>
+      <c r="AV2" s="28"/>
+      <c r="AW2" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="AX2" s="27"/>
-      <c r="AY2" s="27"/>
-      <c r="AZ2" s="27"/>
-      <c r="BA2" s="27"/>
-      <c r="BB2" s="27"/>
-      <c r="BC2" s="27"/>
-      <c r="BD2" s="27" t="s">
+      <c r="AX2" s="28"/>
+      <c r="AY2" s="28"/>
+      <c r="AZ2" s="28"/>
+      <c r="BA2" s="28"/>
+      <c r="BB2" s="28"/>
+      <c r="BC2" s="28"/>
+      <c r="BD2" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="BE2" s="27"/>
-      <c r="BF2" s="27"/>
-      <c r="BG2" s="27"/>
-      <c r="BH2" s="27"/>
-      <c r="BI2" s="27" t="s">
+      <c r="BE2" s="28"/>
+      <c r="BF2" s="28"/>
+      <c r="BG2" s="28"/>
+      <c r="BH2" s="28"/>
+      <c r="BI2" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="BJ2" s="27"/>
-      <c r="BK2" s="27"/>
-      <c r="BL2" s="27"/>
+      <c r="BJ2" s="28"/>
+      <c r="BK2" s="28"/>
+      <c r="BL2" s="28"/>
       <c r="BM2" s="5" t="s">
         <v>47</v>
       </c>
@@ -2678,48 +2678,48 @@
       <c r="J3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="K3" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="30" t="s">
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="30" t="s">
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="V3" s="31"/>
-      <c r="W3" s="31"/>
-      <c r="X3" s="31"/>
-      <c r="Y3" s="32"/>
-      <c r="Z3" s="30" t="s">
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="AA3" s="31"/>
-      <c r="AB3" s="31"/>
-      <c r="AC3" s="31"/>
-      <c r="AD3" s="32"/>
-      <c r="AE3" s="30" t="s">
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="30"/>
+      <c r="AD3" s="31"/>
+      <c r="AE3" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="AF3" s="31"/>
-      <c r="AG3" s="31"/>
-      <c r="AH3" s="31"/>
-      <c r="AI3" s="32"/>
-      <c r="AJ3" s="30" t="s">
+      <c r="AF3" s="30"/>
+      <c r="AG3" s="30"/>
+      <c r="AH3" s="30"/>
+      <c r="AI3" s="31"/>
+      <c r="AJ3" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="AK3" s="31"/>
-      <c r="AL3" s="31"/>
-      <c r="AM3" s="31"/>
-      <c r="AN3" s="32"/>
+      <c r="AK3" s="30"/>
+      <c r="AL3" s="30"/>
+      <c r="AM3" s="30"/>
+      <c r="AN3" s="31"/>
       <c r="AO3" s="3">
         <v>0</v>
       </c>
@@ -2759,10 +2759,10 @@
       <c r="BA3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="BB3" s="28" t="s">
+      <c r="BB3" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="BC3" s="28"/>
+      <c r="BC3" s="33"/>
       <c r="BD3" s="10" t="s">
         <v>57</v>
       </c>
@@ -2772,20 +2772,20 @@
       <c r="BF3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BG3" s="28" t="s">
+      <c r="BG3" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="BH3" s="28"/>
+      <c r="BH3" s="33"/>
       <c r="BI3" s="10" t="s">
         <v>57</v>
       </c>
       <c r="BJ3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BK3" s="28" t="s">
+      <c r="BK3" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="BL3" s="28"/>
+      <c r="BL3" s="33"/>
       <c r="BM3" s="10" t="s">
         <v>1</v>
       </c>
@@ -2816,57 +2816,57 @@
       <c r="K4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="32"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="31"/>
       <c r="P4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="30" t="s">
+      <c r="Q4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="32"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="31"/>
       <c r="U4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="30" t="s">
+      <c r="V4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="31"/>
-      <c r="X4" s="31"/>
-      <c r="Y4" s="32"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="31"/>
       <c r="Z4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AA4" s="30" t="s">
+      <c r="AA4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="31"/>
-      <c r="AC4" s="31"/>
-      <c r="AD4" s="32"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="31"/>
       <c r="AE4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AF4" s="30" t="s">
+      <c r="AF4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AG4" s="31"/>
-      <c r="AH4" s="31"/>
-      <c r="AI4" s="32"/>
+      <c r="AG4" s="30"/>
+      <c r="AH4" s="30"/>
+      <c r="AI4" s="31"/>
       <c r="AJ4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AK4" s="30" t="s">
+      <c r="AK4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AL4" s="31"/>
-      <c r="AM4" s="31"/>
-      <c r="AN4" s="32"/>
+      <c r="AL4" s="30"/>
+      <c r="AM4" s="30"/>
+      <c r="AN4" s="31"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3">
         <v>5</v>
@@ -2969,10 +2969,10 @@
       <c r="M5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="27" t="s">
+      <c r="N5" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="27"/>
+      <c r="O5" s="28"/>
       <c r="P5" s="3">
         <v>7</v>
       </c>
@@ -2982,10 +2982,10 @@
       <c r="R5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="S5" s="27" t="s">
+      <c r="S5" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="T5" s="27"/>
+      <c r="T5" s="28"/>
       <c r="U5" s="3">
         <v>13</v>
       </c>
@@ -2995,10 +2995,10 @@
       <c r="W5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="X5" s="27" t="s">
+      <c r="X5" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="Y5" s="27"/>
+      <c r="Y5" s="28"/>
       <c r="Z5" s="3">
         <v>9</v>
       </c>
@@ -3008,10 +3008,10 @@
       <c r="AB5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AC5" s="27" t="s">
+      <c r="AC5" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="AD5" s="27"/>
+      <c r="AD5" s="28"/>
       <c r="AE5" s="3">
         <v>13</v>
       </c>
@@ -3021,10 +3021,10 @@
       <c r="AG5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AH5" s="27" t="s">
+      <c r="AH5" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="AI5" s="27"/>
+      <c r="AI5" s="28"/>
       <c r="AJ5" s="3">
         <v>9</v>
       </c>
@@ -3034,10 +3034,10 @@
       <c r="AL5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AM5" s="27" t="s">
+      <c r="AM5" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="AN5" s="27"/>
+      <c r="AN5" s="28"/>
       <c r="AO5" s="3"/>
       <c r="AP5" s="3">
         <v>10</v>
@@ -8447,6 +8447,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="AQ2:AV2"/>
+    <mergeCell ref="AW2:BC2"/>
+    <mergeCell ref="BD2:BH2"/>
+    <mergeCell ref="BI2:BL2"/>
+    <mergeCell ref="BB3:BC3"/>
+    <mergeCell ref="AQ1:BM1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I1:AN1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="AO1:AP1"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="N5:O5"/>
@@ -8463,23 +8480,6 @@
     <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="AE3:AI3"/>
     <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AQ1:BM1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I1:AN1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="BG3:BH3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="AQ2:AV2"/>
-    <mergeCell ref="AW2:BC2"/>
-    <mergeCell ref="BD2:BH2"/>
-    <mergeCell ref="BI2:BL2"/>
-    <mergeCell ref="BB3:BC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -8509,26 +8509,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="34" t="s">
+      <c r="F1" s="28"/>
+      <c r="G1" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33" t="s">
+      <c r="H1" s="34"/>
+      <c r="I1" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="33"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -9128,10 +9128,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -9146,175 +9146,175 @@
         <v>3</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="18" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -9326,697 +9326,697 @@
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="16"/>
       <c r="B103" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="16"/>
       <c r="B104" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="16"/>
       <c r="B105" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="16"/>
       <c r="B106" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="16"/>
       <c r="B107" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="16"/>
       <c r="B108" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="16"/>
       <c r="B109" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="16"/>
       <c r="B110" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="16"/>
       <c r="B111" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="16"/>
       <c r="B112" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="16"/>
       <c r="B113" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="16"/>
       <c r="B114" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="16"/>
       <c r="B115" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="16"/>
       <c r="B116" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="16"/>
       <c r="B117" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="16"/>
       <c r="B118" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="16"/>
       <c r="B119" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="16"/>
       <c r="B120" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="16"/>
       <c r="B121" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="16"/>
       <c r="B122" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="16"/>
       <c r="B123" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="16"/>
       <c r="B124" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="16"/>
       <c r="B125" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="16"/>
       <c r="B126" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="16"/>
       <c r="B127" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="16"/>
       <c r="B128" s="26" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="16"/>
       <c r="B129" s="26" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="16"/>
       <c r="B130" s="26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="16"/>
       <c r="B131" s="26" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="16"/>
       <c r="B132" s="26" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="16"/>
       <c r="B133" s="26" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="16"/>
       <c r="B134" s="26" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="16"/>
       <c r="B135" s="26" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="16"/>
       <c r="B136" s="26" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="16"/>
       <c r="B137" s="26" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="16"/>
       <c r="B138" s="26" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="16"/>
       <c r="B139" s="26" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="16"/>
       <c r="B140" s="26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="16"/>
       <c r="B141" s="26" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="16"/>
       <c r="B142" s="26" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="16"/>
       <c r="B143" s="26" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="16"/>
       <c r="B144" s="26" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="16"/>
       <c r="B145" s="26" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="16"/>
       <c r="B146" s="26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="16"/>
       <c r="B147" s="26" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="16"/>
       <c r="B148" s="26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -10032,8 +10032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84235012-AF5A-4BF0-8557-E62F3FAF9D19}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10044,14 +10044,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="A1" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -10060,18 +10060,18 @@
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="36" t="s">
+        <v>221</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="35" t="s">
-        <v>223</v>
-      </c>
-      <c r="F2" s="36"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>91</v>
@@ -10138,7 +10138,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="15" t="s">
-        <v>95</v>
+        <v>251</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="20">
@@ -10152,7 +10152,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="20">
@@ -10166,7 +10166,7 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="20">
@@ -10180,7 +10180,7 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
@@ -10190,7 +10190,7 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -10200,7 +10200,7 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -10210,7 +10210,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="16" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -10245,10 +10245,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -10296,10 +10296,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">

</xml_diff>

<commit_message>
1. Adding code to check space load issues 2. Cleaning up InputJsonData_SpaceLoads.csv 3. Lab space types was wrong in InputJSONData
</commit_message>
<xml_diff>
--- a/data/standards/InputJSONData.xlsx
+++ b/data/standards/InputJSONData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajszi\Documents\openstudio-standards\data\standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3EFA9B-C04D-4A95-8FE0-F935D5E389F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277A0784-D13A-46D6-82A6-CA3203C66A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="5" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
+    <workbookView xWindow="2730" yWindow="1590" windowWidth="21600" windowHeight="11385" tabRatio="868" activeTab="4" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectInformation" sheetId="1" r:id="rId1"/>
@@ -733,9 +733,6 @@
     <t>College-ElevatorShaft</t>
   </si>
   <si>
-    <t>College-EnteranceLobby</t>
-  </si>
-  <si>
     <t>College-Lounge</t>
   </si>
   <si>
@@ -769,18 +766,6 @@
     <t>College-Storage</t>
   </si>
   <si>
-    <t>Lab-Equipment_corridor</t>
-  </si>
-  <si>
-    <t>Lab-Lab_fumehood</t>
-  </si>
-  <si>
-    <t>Lab-Office</t>
-  </si>
-  <si>
-    <t>Lab-Open</t>
-  </si>
-  <si>
     <t>College</t>
   </si>
   <si>
@@ -791,6 +776,21 @@
   </si>
   <si>
     <t>Ideal Loads with Ventilation</t>
+  </si>
+  <si>
+    <t>Laboratory-LabFumeHood</t>
+  </si>
+  <si>
+    <t>Laboratory-OpenLab</t>
+  </si>
+  <si>
+    <t>Laboratory-Office</t>
+  </si>
+  <si>
+    <t>Laboratory-EquipmentCorridor</t>
+  </si>
+  <si>
+    <t>College-Lobby</t>
   </si>
 </sst>
 </file>
@@ -834,9 +834,10 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -846,6 +847,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -939,7 +946,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1010,7 +1017,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1020,12 +1034,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1374,14 +1382,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1515,12 +1523,12 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -1564,10 +1572,10 @@
       <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2469,82 +2477,82 @@
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="29" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="28" t="s">
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="34"/>
+      <c r="AO1" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="AP1" s="28"/>
-      <c r="AQ1" s="32" t="s">
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="32"/>
-      <c r="BC1" s="32"/>
-      <c r="BD1" s="32"/>
-      <c r="BE1" s="32"/>
-      <c r="BF1" s="32"/>
-      <c r="BG1" s="32"/>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
-      <c r="BK1" s="32"/>
-      <c r="BL1" s="32"/>
-      <c r="BM1" s="32"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
+      <c r="AW1" s="31"/>
+      <c r="AX1" s="31"/>
+      <c r="AY1" s="31"/>
+      <c r="AZ1" s="31"/>
+      <c r="BA1" s="31"/>
+      <c r="BB1" s="31"/>
+      <c r="BC1" s="31"/>
+      <c r="BD1" s="31"/>
+      <c r="BE1" s="31"/>
+      <c r="BF1" s="31"/>
+      <c r="BG1" s="31"/>
+      <c r="BH1" s="31"/>
+      <c r="BI1" s="31"/>
+      <c r="BJ1" s="31"/>
+      <c r="BK1" s="31"/>
+      <c r="BL1" s="31"/>
+      <c r="BM1" s="31"/>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2562,10 +2570,10 @@
       <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="28"/>
+      <c r="G2" s="29"/>
       <c r="H2" s="25" t="s">
         <v>223</v>
       </c>
@@ -2575,74 +2583,74 @@
       <c r="J2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="28"/>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28"/>
-      <c r="AE2" s="28"/>
-      <c r="AF2" s="28"/>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="28"/>
-      <c r="AN2" s="28"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29"/>
+      <c r="AH2" s="29"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29"/>
       <c r="AO2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AP2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AQ2" s="28" t="s">
+      <c r="AQ2" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="AR2" s="28"/>
-      <c r="AS2" s="28"/>
-      <c r="AT2" s="28"/>
-      <c r="AU2" s="28"/>
-      <c r="AV2" s="28"/>
-      <c r="AW2" s="28" t="s">
+      <c r="AR2" s="29"/>
+      <c r="AS2" s="29"/>
+      <c r="AT2" s="29"/>
+      <c r="AU2" s="29"/>
+      <c r="AV2" s="29"/>
+      <c r="AW2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="AX2" s="28"/>
-      <c r="AY2" s="28"/>
-      <c r="AZ2" s="28"/>
-      <c r="BA2" s="28"/>
-      <c r="BB2" s="28"/>
-      <c r="BC2" s="28"/>
-      <c r="BD2" s="28" t="s">
+      <c r="AX2" s="29"/>
+      <c r="AY2" s="29"/>
+      <c r="AZ2" s="29"/>
+      <c r="BA2" s="29"/>
+      <c r="BB2" s="29"/>
+      <c r="BC2" s="29"/>
+      <c r="BD2" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="BE2" s="28"/>
-      <c r="BF2" s="28"/>
-      <c r="BG2" s="28"/>
-      <c r="BH2" s="28"/>
-      <c r="BI2" s="28" t="s">
+      <c r="BE2" s="29"/>
+      <c r="BF2" s="29"/>
+      <c r="BG2" s="29"/>
+      <c r="BH2" s="29"/>
+      <c r="BI2" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="BJ2" s="28"/>
-      <c r="BK2" s="28"/>
-      <c r="BL2" s="28"/>
+      <c r="BJ2" s="29"/>
+      <c r="BK2" s="29"/>
+      <c r="BL2" s="29"/>
       <c r="BM2" s="5" t="s">
         <v>47</v>
       </c>
@@ -2678,48 +2686,48 @@
       <c r="J3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="29" t="s">
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="29" t="s">
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="31"/>
-      <c r="Z3" s="29" t="s">
+      <c r="V3" s="33"/>
+      <c r="W3" s="33"/>
+      <c r="X3" s="33"/>
+      <c r="Y3" s="34"/>
+      <c r="Z3" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="30"/>
-      <c r="AD3" s="31"/>
-      <c r="AE3" s="29" t="s">
+      <c r="AA3" s="33"/>
+      <c r="AB3" s="33"/>
+      <c r="AC3" s="33"/>
+      <c r="AD3" s="34"/>
+      <c r="AE3" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="AF3" s="30"/>
-      <c r="AG3" s="30"/>
-      <c r="AH3" s="30"/>
-      <c r="AI3" s="31"/>
-      <c r="AJ3" s="29" t="s">
+      <c r="AF3" s="33"/>
+      <c r="AG3" s="33"/>
+      <c r="AH3" s="33"/>
+      <c r="AI3" s="34"/>
+      <c r="AJ3" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="AK3" s="30"/>
-      <c r="AL3" s="30"/>
-      <c r="AM3" s="30"/>
-      <c r="AN3" s="31"/>
+      <c r="AK3" s="33"/>
+      <c r="AL3" s="33"/>
+      <c r="AM3" s="33"/>
+      <c r="AN3" s="34"/>
       <c r="AO3" s="3">
         <v>0</v>
       </c>
@@ -2759,10 +2767,10 @@
       <c r="BA3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="BB3" s="33" t="s">
+      <c r="BB3" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="BC3" s="33"/>
+      <c r="BC3" s="30"/>
       <c r="BD3" s="10" t="s">
         <v>57</v>
       </c>
@@ -2772,20 +2780,20 @@
       <c r="BF3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BG3" s="33" t="s">
+      <c r="BG3" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="BH3" s="33"/>
+      <c r="BH3" s="30"/>
       <c r="BI3" s="10" t="s">
         <v>57</v>
       </c>
       <c r="BJ3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BK3" s="33" t="s">
+      <c r="BK3" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="BL3" s="33"/>
+      <c r="BL3" s="30"/>
       <c r="BM3" s="10" t="s">
         <v>1</v>
       </c>
@@ -2816,57 +2824,57 @@
       <c r="K4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="29" t="s">
+      <c r="L4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="31"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="34"/>
       <c r="P4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="29" t="s">
+      <c r="Q4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="31"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="34"/>
       <c r="U4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="29" t="s">
+      <c r="V4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="31"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="34"/>
       <c r="Z4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AA4" s="29" t="s">
+      <c r="AA4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="31"/>
+      <c r="AB4" s="33"/>
+      <c r="AC4" s="33"/>
+      <c r="AD4" s="34"/>
       <c r="AE4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AF4" s="29" t="s">
+      <c r="AF4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="AG4" s="30"/>
-      <c r="AH4" s="30"/>
-      <c r="AI4" s="31"/>
+      <c r="AG4" s="33"/>
+      <c r="AH4" s="33"/>
+      <c r="AI4" s="34"/>
       <c r="AJ4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AK4" s="29" t="s">
+      <c r="AK4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="AL4" s="30"/>
-      <c r="AM4" s="30"/>
-      <c r="AN4" s="31"/>
+      <c r="AL4" s="33"/>
+      <c r="AM4" s="33"/>
+      <c r="AN4" s="34"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3">
         <v>5</v>
@@ -2969,10 +2977,10 @@
       <c r="M5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="28" t="s">
+      <c r="N5" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="28"/>
+      <c r="O5" s="29"/>
       <c r="P5" s="3">
         <v>7</v>
       </c>
@@ -2982,10 +2990,10 @@
       <c r="R5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="S5" s="28" t="s">
+      <c r="S5" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="T5" s="28"/>
+      <c r="T5" s="29"/>
       <c r="U5" s="3">
         <v>13</v>
       </c>
@@ -2995,10 +3003,10 @@
       <c r="W5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="X5" s="28" t="s">
+      <c r="X5" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="Y5" s="28"/>
+      <c r="Y5" s="29"/>
       <c r="Z5" s="3">
         <v>9</v>
       </c>
@@ -3008,10 +3016,10 @@
       <c r="AB5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AC5" s="28" t="s">
+      <c r="AC5" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="AD5" s="28"/>
+      <c r="AD5" s="29"/>
       <c r="AE5" s="3">
         <v>13</v>
       </c>
@@ -3021,10 +3029,10 @@
       <c r="AG5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AH5" s="28" t="s">
+      <c r="AH5" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="AI5" s="28"/>
+      <c r="AI5" s="29"/>
       <c r="AJ5" s="3">
         <v>9</v>
       </c>
@@ -3034,10 +3042,10 @@
       <c r="AL5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AM5" s="28" t="s">
+      <c r="AM5" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="AN5" s="28"/>
+      <c r="AN5" s="29"/>
       <c r="AO5" s="3"/>
       <c r="AP5" s="3">
         <v>10</v>
@@ -8447,23 +8455,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="BG3:BH3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="AQ2:AV2"/>
-    <mergeCell ref="AW2:BC2"/>
-    <mergeCell ref="BD2:BH2"/>
-    <mergeCell ref="BI2:BL2"/>
-    <mergeCell ref="BB3:BC3"/>
-    <mergeCell ref="AQ1:BM1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I1:AN1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="AO1:AP1"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="N5:O5"/>
@@ -8480,6 +8471,23 @@
     <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="AE3:AI3"/>
     <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AQ1:BM1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I1:AN1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="AQ2:AV2"/>
+    <mergeCell ref="AW2:BC2"/>
+    <mergeCell ref="BD2:BH2"/>
+    <mergeCell ref="BI2:BL2"/>
+    <mergeCell ref="BB3:BC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -8509,26 +8517,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="35" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34" t="s">
+      <c r="H1" s="35"/>
+      <c r="I1" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="34"/>
+      <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -9116,8 +9124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C609DAD-BC63-4626-ACCC-69F8C32CB7AB}">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B143" sqref="B143"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9128,10 +9136,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="34"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -9914,43 +9922,43 @@
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="16"/>
       <c r="B131" s="26" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="16"/>
       <c r="B132" s="26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="16"/>
       <c r="B133" s="26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="16"/>
       <c r="B134" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="16"/>
       <c r="B135" s="26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="16"/>
       <c r="B136" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="16"/>
       <c r="B137" s="26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -9968,55 +9976,55 @@
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="16"/>
       <c r="B140" s="26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="16"/>
       <c r="B141" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="16"/>
       <c r="B142" s="26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="16"/>
       <c r="B143" s="26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="16"/>
       <c r="B144" s="26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="16"/>
-      <c r="B145" s="26" t="s">
-        <v>245</v>
+      <c r="B145" s="28" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="16"/>
-      <c r="B146" s="26" t="s">
-        <v>246</v>
+      <c r="B146" s="28" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="16"/>
-      <c r="B147" s="26" t="s">
-        <v>247</v>
+      <c r="B147" s="28" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="16"/>
-      <c r="B148" s="26" t="s">
-        <v>248</v>
+      <c r="B148" s="28" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -10032,7 +10040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84235012-AF5A-4BF0-8557-E62F3FAF9D19}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -10044,14 +10052,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>224</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -10060,14 +10068,14 @@
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="36" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="37" t="s">
         <v>222</v>
       </c>
-      <c r="F2" s="37"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -10138,7 +10146,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="15" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="20">
@@ -10210,7 +10218,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="16" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -10245,10 +10253,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -10296,10 +10304,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">

</xml_diff>